<commit_message>
Added Roadmap of Secret Sharing to Gantt Chart
</commit_message>
<xml_diff>
--- a/docs/gantt_chart_secrecy.xlsx
+++ b/docs/gantt_chart_secrecy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evonik-my.sharepoint.com/personal/d23031_evonik_com/Documents/Dokumente/personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mimoun.mendoughe/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{231D11F1-127A-461E-8A03-FE34AE8E1065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE6CE7D-10DB-7145-9EF1-483A4AF486A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D30480B8-D58C-44F1-852C-2B52D77C9917}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30940" windowHeight="16780" xr2:uid="{D30480B8-D58C-44F1-852C-2B52D77C9917}"/>
   </bookViews>
   <sheets>
     <sheet name="Mappe 1" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="43">
   <si>
     <t>FESCA Project</t>
   </si>
@@ -142,13 +142,34 @@
     <t>2 MPC Runtime and oblivious operators</t>
   </si>
   <si>
-    <t>3 Secret Sharing and data ingestion</t>
-  </si>
-  <si>
     <t>4 MPC Protocol layer</t>
   </si>
   <si>
     <t>KW 27 (June-July)</t>
+  </si>
+  <si>
+    <t>3a Interface for Uploading tables</t>
+  </si>
+  <si>
+    <t>3b Row Reader &amp; Bit String Encoder</t>
+  </si>
+  <si>
+    <t>3c Generating shares for tuple</t>
+  </si>
+  <si>
+    <t>3d Generating shares of a table</t>
+  </si>
+  <si>
+    <t>3e Setting up the receive procedure</t>
+  </si>
+  <si>
+    <t>3 Secret Sharing and data ingestion (Mimoun)</t>
+  </si>
+  <si>
+    <t>3f Integration</t>
+  </si>
+  <si>
+    <t>3g testing</t>
   </si>
 </sst>
 </file>
@@ -156,10 +177,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;€&quot;* #,##0.00_);_(&quot;€&quot;* \(#,##0.00\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;€&quot;* #,##0.00_);_(&quot;€&quot;* \(#,##0.00\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -619,9 +640,9 @@
   </borders>
   <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" applyFill="0" applyProtection="0">
@@ -652,7 +673,7 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -672,28 +693,19 @@
     <xf numFmtId="0" fontId="19" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -703,20 +715,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -728,24 +734,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -754,7 +757,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Accent1" xfId="22" builtinId="29" customBuiltin="1"/>
@@ -2022,258 +2035,257 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:DP31"/>
+  <dimension ref="A1:DP32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="BB21" sqref="BB21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.90625" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="1.36328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="1.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="1.36328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="1.453125" style="32" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="1.6328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="1.36328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="1.81640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="37" max="41" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="44" max="48" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="51" max="54" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="1.36328125" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="1.453125" style="32" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="1.6328125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="1.36328125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="1.81640625" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="1.36328125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="1.453125" style="32" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="65" max="69" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="72" max="76" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="77" max="78" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="79" max="83" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="84" max="85" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="1.6328125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="1.36328125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="1.81640625" bestFit="1" customWidth="1"/>
-    <col min="89" max="90" width="1.36328125" bestFit="1" customWidth="1"/>
-    <col min="91" max="92" width="1.453125" style="32" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="1.6328125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="1.36328125" bestFit="1" customWidth="1"/>
-    <col min="95" max="97" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="98" max="99" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="100" max="104" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="105" max="106" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="108" max="109" width="1.90625" style="15" bestFit="1" customWidth="1"/>
-    <col min="110" max="111" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="112" max="113" width="1.90625" style="32" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="1.90625" style="12" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="1.81640625" bestFit="1" customWidth="1"/>
-    <col min="117" max="118" width="1.36328125" bestFit="1" customWidth="1"/>
-    <col min="119" max="120" width="1.453125" style="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="1.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="37" max="41" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="44" max="48" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="51" max="54" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="1.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="1.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="65" max="69" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="72" max="76" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="79" max="83" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="84" max="85" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="89" max="90" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="91" max="92" width="1.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="95" max="97" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="98" max="99" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="100" max="104" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="105" max="106" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="108" max="109" width="1.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="110" max="111" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="112" max="113" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="1.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="117" max="118" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="119" max="120" width="1.42578125" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="F1" s="45"/>
-      <c r="DD1" s="20"/>
-      <c r="DE1" s="20"/>
-      <c r="DK1" s="20"/>
+      <c r="F1" s="33"/>
+      <c r="DD1"/>
+      <c r="DE1"/>
+      <c r="DK1"/>
     </row>
-    <row r="2" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="DD2" s="20"/>
-      <c r="DE2" s="20"/>
-      <c r="DK2" s="20"/>
+      <c r="DD2"/>
+      <c r="DE2"/>
+      <c r="DK2"/>
     </row>
-    <row r="3" spans="1:120" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:120" ht="19" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="DD3" s="20"/>
-      <c r="DE3" s="20"/>
-      <c r="DK3" s="20"/>
+      <c r="DD3"/>
+      <c r="DE3"/>
+      <c r="DK3"/>
     </row>
-    <row r="4" spans="1:120" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:120" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="9" t="s">
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="9" t="s">
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="42"/>
+      <c r="AD4" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="7"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="9" t="s">
+      <c r="AE4" s="41"/>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="41"/>
+      <c r="AH4" s="41"/>
+      <c r="AI4" s="41"/>
+      <c r="AJ4" s="42"/>
+      <c r="AK4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="AL4" s="7"/>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="7"/>
-      <c r="AQ4" s="8"/>
-      <c r="AR4" s="9" t="s">
+      <c r="AL4" s="41"/>
+      <c r="AM4" s="41"/>
+      <c r="AN4" s="41"/>
+      <c r="AO4" s="41"/>
+      <c r="AP4" s="41"/>
+      <c r="AQ4" s="42"/>
+      <c r="AR4" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="7"/>
-      <c r="AU4" s="7"/>
-      <c r="AV4" s="7"/>
-      <c r="AW4" s="7"/>
-      <c r="AX4" s="8"/>
-      <c r="AY4" s="9" t="s">
+      <c r="AS4" s="41"/>
+      <c r="AT4" s="41"/>
+      <c r="AU4" s="41"/>
+      <c r="AV4" s="41"/>
+      <c r="AW4" s="41"/>
+      <c r="AX4" s="42"/>
+      <c r="AY4" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="AZ4" s="7"/>
-      <c r="BA4" s="7"/>
-      <c r="BB4" s="7"/>
-      <c r="BC4" s="7"/>
-      <c r="BD4" s="7"/>
-      <c r="BE4" s="8"/>
-      <c r="BF4" s="9" t="s">
+      <c r="AZ4" s="41"/>
+      <c r="BA4" s="41"/>
+      <c r="BB4" s="41"/>
+      <c r="BC4" s="41"/>
+      <c r="BD4" s="41"/>
+      <c r="BE4" s="42"/>
+      <c r="BF4" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="BG4" s="7"/>
-      <c r="BH4" s="7"/>
-      <c r="BI4" s="7"/>
-      <c r="BJ4" s="7"/>
-      <c r="BK4" s="7"/>
-      <c r="BL4" s="8"/>
-      <c r="BM4" s="9" t="s">
+      <c r="BG4" s="41"/>
+      <c r="BH4" s="41"/>
+      <c r="BI4" s="41"/>
+      <c r="BJ4" s="41"/>
+      <c r="BK4" s="41"/>
+      <c r="BL4" s="42"/>
+      <c r="BM4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="BN4" s="7"/>
-      <c r="BO4" s="7"/>
-      <c r="BP4" s="7"/>
-      <c r="BQ4" s="7"/>
-      <c r="BR4" s="7"/>
-      <c r="BS4" s="8"/>
-      <c r="BT4" s="9" t="s">
+      <c r="BN4" s="41"/>
+      <c r="BO4" s="41"/>
+      <c r="BP4" s="41"/>
+      <c r="BQ4" s="41"/>
+      <c r="BR4" s="41"/>
+      <c r="BS4" s="42"/>
+      <c r="BT4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="BU4" s="7"/>
-      <c r="BV4" s="7"/>
-      <c r="BW4" s="7"/>
-      <c r="BX4" s="7"/>
-      <c r="BY4" s="7"/>
-      <c r="BZ4" s="8"/>
-      <c r="CA4" s="9" t="s">
+      <c r="BU4" s="41"/>
+      <c r="BV4" s="41"/>
+      <c r="BW4" s="41"/>
+      <c r="BX4" s="41"/>
+      <c r="BY4" s="41"/>
+      <c r="BZ4" s="42"/>
+      <c r="CA4" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="CB4" s="7"/>
-      <c r="CC4" s="7"/>
-      <c r="CD4" s="7"/>
-      <c r="CE4" s="7"/>
-      <c r="CF4" s="7"/>
-      <c r="CG4" s="8"/>
-      <c r="CH4" s="9" t="s">
+      <c r="CB4" s="41"/>
+      <c r="CC4" s="41"/>
+      <c r="CD4" s="41"/>
+      <c r="CE4" s="41"/>
+      <c r="CF4" s="41"/>
+      <c r="CG4" s="42"/>
+      <c r="CH4" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="CI4" s="7"/>
-      <c r="CJ4" s="7"/>
-      <c r="CK4" s="7"/>
-      <c r="CL4" s="7"/>
-      <c r="CM4" s="7"/>
-      <c r="CN4" s="8"/>
-      <c r="CO4" s="9" t="s">
+      <c r="CI4" s="41"/>
+      <c r="CJ4" s="41"/>
+      <c r="CK4" s="41"/>
+      <c r="CL4" s="41"/>
+      <c r="CM4" s="41"/>
+      <c r="CN4" s="42"/>
+      <c r="CO4" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="CP4" s="7"/>
-      <c r="CQ4" s="7"/>
-      <c r="CR4" s="7"/>
-      <c r="CS4" s="7"/>
-      <c r="CT4" s="7"/>
-      <c r="CU4" s="8"/>
-      <c r="CV4" s="9" t="s">
+      <c r="CP4" s="41"/>
+      <c r="CQ4" s="41"/>
+      <c r="CR4" s="41"/>
+      <c r="CS4" s="41"/>
+      <c r="CT4" s="41"/>
+      <c r="CU4" s="42"/>
+      <c r="CV4" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="CW4" s="7"/>
-      <c r="CX4" s="7"/>
-      <c r="CY4" s="7"/>
-      <c r="CZ4" s="7"/>
-      <c r="DA4" s="7"/>
-      <c r="DB4" s="8"/>
-      <c r="DC4" s="9" t="s">
+      <c r="CW4" s="41"/>
+      <c r="CX4" s="41"/>
+      <c r="CY4" s="41"/>
+      <c r="CZ4" s="41"/>
+      <c r="DA4" s="41"/>
+      <c r="DB4" s="42"/>
+      <c r="DC4" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="DD4" s="7"/>
-      <c r="DE4" s="7"/>
-      <c r="DF4" s="7"/>
-      <c r="DG4" s="7"/>
-      <c r="DH4" s="7"/>
-      <c r="DI4" s="8"/>
-      <c r="DJ4" s="9" t="s">
+      <c r="DD4" s="41"/>
+      <c r="DE4" s="41"/>
+      <c r="DF4" s="41"/>
+      <c r="DG4" s="41"/>
+      <c r="DH4" s="41"/>
+      <c r="DI4" s="42"/>
+      <c r="DJ4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="DK4" s="7"/>
-      <c r="DL4" s="7"/>
-      <c r="DM4" s="7"/>
-      <c r="DN4" s="7"/>
-      <c r="DO4" s="7"/>
-      <c r="DP4" s="8"/>
+      <c r="DK4" s="41"/>
+      <c r="DL4" s="41"/>
+      <c r="DM4" s="41"/>
+      <c r="DN4" s="41"/>
+      <c r="DO4" s="41"/>
+      <c r="DP4" s="42"/>
     </row>
-    <row r="5" spans="1:120" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:120" ht="19" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="2">
         <v>9</v>
@@ -2287,13 +2299,13 @@
       <c r="E5" s="2">
         <v>12</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="35">
         <v>13</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="24">
         <v>14</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="25">
         <v>15</v>
       </c>
       <c r="I5" s="3">
@@ -2311,10 +2323,10 @@
       <c r="M5" s="2">
         <v>20</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="24">
         <v>21</v>
       </c>
-      <c r="O5" s="34">
+      <c r="O5" s="25">
         <v>22</v>
       </c>
       <c r="P5" s="3">
@@ -2332,10 +2344,10 @@
       <c r="T5" s="2">
         <v>27</v>
       </c>
-      <c r="U5" s="33">
+      <c r="U5" s="24">
         <v>28</v>
       </c>
-      <c r="V5" s="34">
+      <c r="V5" s="25">
         <v>29</v>
       </c>
       <c r="W5" s="3">
@@ -2353,10 +2365,10 @@
       <c r="AA5" s="2">
         <v>4</v>
       </c>
-      <c r="AB5" s="33">
+      <c r="AB5" s="24">
         <v>5</v>
       </c>
-      <c r="AC5" s="34">
+      <c r="AC5" s="25">
         <v>6</v>
       </c>
       <c r="AD5" s="3">
@@ -2374,10 +2386,10 @@
       <c r="AH5" s="2">
         <v>11</v>
       </c>
-      <c r="AI5" s="33">
+      <c r="AI5" s="24">
         <v>12</v>
       </c>
-      <c r="AJ5" s="34">
+      <c r="AJ5" s="25">
         <v>13</v>
       </c>
       <c r="AK5" s="3">
@@ -2395,10 +2407,10 @@
       <c r="AO5" s="2">
         <v>18</v>
       </c>
-      <c r="AP5" s="33">
+      <c r="AP5" s="24">
         <v>19</v>
       </c>
-      <c r="AQ5" s="34">
+      <c r="AQ5" s="25">
         <v>20</v>
       </c>
       <c r="AR5" s="3">
@@ -2416,10 +2428,10 @@
       <c r="AV5" s="2">
         <v>25</v>
       </c>
-      <c r="AW5" s="33">
+      <c r="AW5" s="24">
         <v>26</v>
       </c>
-      <c r="AX5" s="34">
+      <c r="AX5" s="25">
         <v>27</v>
       </c>
       <c r="AY5" s="3">
@@ -2437,10 +2449,10 @@
       <c r="BC5" s="2">
         <v>1</v>
       </c>
-      <c r="BD5" s="33">
+      <c r="BD5" s="24">
         <v>2</v>
       </c>
-      <c r="BE5" s="33">
+      <c r="BE5" s="24">
         <v>3</v>
       </c>
       <c r="BF5" s="2">
@@ -2458,10 +2470,10 @@
       <c r="BJ5" s="2">
         <v>8</v>
       </c>
-      <c r="BK5" s="33">
+      <c r="BK5" s="24">
         <v>9</v>
       </c>
-      <c r="BL5" s="33">
+      <c r="BL5" s="24">
         <v>10</v>
       </c>
       <c r="BM5" s="2">
@@ -2479,10 +2491,10 @@
       <c r="BQ5" s="2">
         <v>15</v>
       </c>
-      <c r="BR5" s="33">
+      <c r="BR5" s="24">
         <v>16</v>
       </c>
-      <c r="BS5" s="33">
+      <c r="BS5" s="24">
         <v>17</v>
       </c>
       <c r="BT5" s="2">
@@ -2500,10 +2512,10 @@
       <c r="BX5" s="2">
         <v>22</v>
       </c>
-      <c r="BY5" s="33">
+      <c r="BY5" s="24">
         <v>23</v>
       </c>
-      <c r="BZ5" s="33">
+      <c r="BZ5" s="24">
         <v>24</v>
       </c>
       <c r="CA5" s="2">
@@ -2521,104 +2533,104 @@
       <c r="CE5" s="2">
         <v>29</v>
       </c>
-      <c r="CF5" s="33">
+      <c r="CF5" s="24">
         <v>30</v>
       </c>
-      <c r="CG5" s="33">
+      <c r="CG5" s="24">
         <v>31</v>
       </c>
-      <c r="CH5" s="11">
+      <c r="CH5" s="8">
         <v>1</v>
       </c>
-      <c r="CI5" s="11">
+      <c r="CI5" s="8">
         <v>2</v>
       </c>
-      <c r="CJ5" s="11">
+      <c r="CJ5" s="8">
         <v>3</v>
       </c>
-      <c r="CK5" s="11">
+      <c r="CK5" s="8">
         <v>4</v>
       </c>
-      <c r="CL5" s="11">
+      <c r="CL5" s="8">
         <v>5</v>
       </c>
-      <c r="CM5" s="41">
+      <c r="CM5" s="30">
         <v>6</v>
       </c>
-      <c r="CN5" s="41">
+      <c r="CN5" s="30">
         <v>7</v>
       </c>
-      <c r="CO5" s="11">
+      <c r="CO5" s="8">
         <v>8</v>
       </c>
-      <c r="CP5" s="11">
+      <c r="CP5" s="8">
         <v>9</v>
       </c>
-      <c r="CQ5" s="11">
+      <c r="CQ5" s="8">
         <v>10</v>
       </c>
-      <c r="CR5" s="11">
+      <c r="CR5" s="8">
         <v>11</v>
       </c>
-      <c r="CS5" s="11">
+      <c r="CS5" s="8">
         <v>12</v>
       </c>
-      <c r="CT5" s="41">
+      <c r="CT5" s="30">
         <v>13</v>
       </c>
-      <c r="CU5" s="41">
+      <c r="CU5" s="30">
         <v>14</v>
       </c>
-      <c r="CV5" s="11">
+      <c r="CV5" s="8">
         <v>15</v>
       </c>
-      <c r="CW5" s="11">
+      <c r="CW5" s="8">
         <v>16</v>
       </c>
-      <c r="CX5" s="11">
+      <c r="CX5" s="8">
         <v>17</v>
       </c>
-      <c r="CY5" s="11">
+      <c r="CY5" s="8">
         <v>18</v>
       </c>
-      <c r="CZ5" s="11">
+      <c r="CZ5" s="8">
         <v>19</v>
       </c>
-      <c r="DA5" s="41">
+      <c r="DA5" s="30">
         <v>20</v>
       </c>
-      <c r="DB5" s="41">
+      <c r="DB5" s="30">
         <v>21</v>
       </c>
-      <c r="DC5" s="11">
+      <c r="DC5" s="8">
         <v>22</v>
       </c>
-      <c r="DD5" s="16">
+      <c r="DD5" s="13">
         <v>23</v>
       </c>
-      <c r="DE5" s="16">
+      <c r="DE5" s="13">
         <v>24</v>
       </c>
-      <c r="DF5" s="11">
+      <c r="DF5" s="8">
         <v>25</v>
       </c>
-      <c r="DG5" s="11">
+      <c r="DG5" s="8">
         <v>26</v>
       </c>
-      <c r="DH5" s="41">
+      <c r="DH5" s="30">
         <v>27</v>
       </c>
-      <c r="DI5" s="41">
+      <c r="DI5" s="30">
         <v>28</v>
       </c>
-      <c r="DJ5" s="11">
+      <c r="DJ5" s="8">
         <v>29</v>
       </c>
-      <c r="DK5" s="13">
+      <c r="DK5" s="10">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:120" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:120" ht="19" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="4" t="s">
         <v>1</v>
@@ -2632,13 +2644,13 @@
       <c r="E6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="5" t="s">
@@ -2656,10 +2668,10 @@
       <c r="M6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="35" t="s">
+      <c r="N6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="P6" s="5" t="s">
@@ -2677,10 +2689,10 @@
       <c r="T6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="U6" s="35" t="s">
+      <c r="U6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="V6" s="35" t="s">
+      <c r="V6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="W6" s="5" t="s">
@@ -2698,10 +2710,10 @@
       <c r="AA6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AB6" s="35" t="s">
+      <c r="AB6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AC6" s="35" t="s">
+      <c r="AC6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="AD6" s="5" t="s">
@@ -2719,10 +2731,10 @@
       <c r="AH6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AI6" s="35" t="s">
+      <c r="AI6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AJ6" s="35" t="s">
+      <c r="AJ6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="AK6" s="5" t="s">
@@ -2740,10 +2752,10 @@
       <c r="AO6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AP6" s="35" t="s">
+      <c r="AP6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AQ6" s="35" t="s">
+      <c r="AQ6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="AR6" s="5" t="s">
@@ -2761,10 +2773,10 @@
       <c r="AV6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AW6" s="35" t="s">
+      <c r="AW6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AX6" s="35" t="s">
+      <c r="AX6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="AY6" s="5" t="s">
@@ -2782,10 +2794,10 @@
       <c r="BC6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BD6" s="35" t="s">
+      <c r="BD6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="BE6" s="40" t="s">
+      <c r="BE6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="BF6" s="5" t="s">
@@ -2803,10 +2815,10 @@
       <c r="BJ6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BK6" s="35" t="s">
+      <c r="BK6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="BL6" s="40" t="s">
+      <c r="BL6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="BM6" s="5" t="s">
@@ -2824,10 +2836,10 @@
       <c r="BQ6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BR6" s="35" t="s">
+      <c r="BR6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="BS6" s="40" t="s">
+      <c r="BS6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="BT6" s="5" t="s">
@@ -2845,10 +2857,10 @@
       <c r="BX6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BY6" s="35" t="s">
+      <c r="BY6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="BZ6" s="40" t="s">
+      <c r="BZ6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="CA6" s="5" t="s">
@@ -2866,10 +2878,10 @@
       <c r="CE6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="CF6" s="35" t="s">
+      <c r="CF6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="CG6" s="40" t="s">
+      <c r="CG6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="CH6" s="5" t="s">
@@ -2887,10 +2899,10 @@
       <c r="CL6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="CM6" s="35" t="s">
+      <c r="CM6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="CN6" s="40" t="s">
+      <c r="CN6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="CO6" s="5" t="s">
@@ -2908,10 +2920,10 @@
       <c r="CS6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="CT6" s="35" t="s">
+      <c r="CT6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="CU6" s="40" t="s">
+      <c r="CU6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="CV6" s="5" t="s">
@@ -2929,19 +2941,19 @@
       <c r="CZ6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="DA6" s="35" t="s">
+      <c r="DA6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="DB6" s="40" t="s">
+      <c r="DB6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="DC6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="DD6" s="17" t="s">
+      <c r="DD6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="DE6" s="17" t="s">
+      <c r="DE6" s="14" t="s">
         <v>3</v>
       </c>
       <c r="DF6" s="5" t="s">
@@ -2950,16 +2962,16 @@
       <c r="DG6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="DH6" s="35" t="s">
+      <c r="DH6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="DI6" s="40" t="s">
+      <c r="DI6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="DJ6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="DK6" s="14" t="s">
+      <c r="DK6" s="11" t="s">
         <v>2</v>
       </c>
       <c r="DL6" s="5" t="s">
@@ -2971,368 +2983,459 @@
       <c r="DN6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="DO6" s="35" t="s">
+      <c r="DO6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="DP6" s="40" t="s">
+      <c r="DP6" s="29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:120" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+    <row r="7" spans="1:120" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="F7" s="49"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="F7" s="37"/>
     </row>
-    <row r="8" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="AV8" s="10"/>
-      <c r="AW8" s="10"/>
-      <c r="AX8" s="10"/>
-      <c r="AY8" s="10"/>
-      <c r="AZ8" s="10"/>
-      <c r="BA8" s="10"/>
-      <c r="BB8" s="10"/>
-      <c r="BC8" s="10"/>
-      <c r="BF8" s="10"/>
-      <c r="BG8" s="10"/>
-      <c r="BH8" s="10"/>
-      <c r="BI8" s="10"/>
-      <c r="BJ8" s="10"/>
-      <c r="BM8" s="10"/>
-      <c r="BN8" s="10"/>
-      <c r="BO8" s="10"/>
-      <c r="BP8" s="10"/>
-      <c r="BQ8" s="10"/>
-      <c r="BT8" s="10"/>
-      <c r="BU8" s="10"/>
-      <c r="BV8" s="10"/>
-      <c r="BW8" s="10"/>
-      <c r="BX8" s="10"/>
+      <c r="AV8" s="7"/>
+      <c r="AW8" s="7"/>
+      <c r="AX8" s="7"/>
+      <c r="AY8" s="7"/>
+      <c r="AZ8" s="7"/>
+      <c r="BA8" s="7"/>
+      <c r="BB8" s="7"/>
+      <c r="BC8" s="7"/>
+      <c r="BF8" s="7"/>
+      <c r="BG8" s="7"/>
+      <c r="BH8" s="7"/>
+      <c r="BI8" s="7"/>
+      <c r="BJ8" s="7"/>
+      <c r="BM8" s="7"/>
+      <c r="BN8" s="7"/>
+      <c r="BO8" s="7"/>
+      <c r="BP8" s="7"/>
+      <c r="BQ8" s="7"/>
+      <c r="BT8" s="7"/>
+      <c r="BU8" s="7"/>
+      <c r="BV8" s="7"/>
+      <c r="BW8" s="7"/>
+      <c r="BX8" s="7"/>
     </row>
-    <row r="9" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="10"/>
-      <c r="AF9" s="10"/>
-      <c r="AG9" s="10"/>
-      <c r="AH9" s="10"/>
-      <c r="AK9" s="10"/>
-      <c r="AL9" s="10"/>
-      <c r="AM9" s="10"/>
-      <c r="AN9" s="10"/>
-      <c r="AO9" s="10"/>
-      <c r="AR9" s="10"/>
-      <c r="AS9" s="10"/>
-      <c r="AT9" s="10"/>
-      <c r="AU9" s="10"/>
-      <c r="AV9" s="10"/>
-      <c r="AW9" s="10"/>
-      <c r="AX9" s="10"/>
-      <c r="AY9" s="10"/>
-      <c r="AZ9" s="10"/>
-      <c r="BA9" s="10"/>
-      <c r="BB9" s="10"/>
-      <c r="BC9" s="10"/>
-      <c r="BF9" s="10"/>
-      <c r="BG9" s="10"/>
-      <c r="BH9" s="10"/>
-      <c r="BI9" s="10"/>
-      <c r="BJ9" s="10"/>
-      <c r="BM9" s="10"/>
-      <c r="BN9" s="10"/>
-      <c r="BO9" s="10"/>
-      <c r="BP9" s="10"/>
-      <c r="BQ9" s="10"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AK9" s="7"/>
+      <c r="AL9" s="7"/>
+      <c r="AM9" s="7"/>
+      <c r="AN9" s="7"/>
+      <c r="AO9" s="7"/>
+      <c r="AR9" s="7"/>
+      <c r="AS9" s="7"/>
+      <c r="AT9" s="7"/>
+      <c r="AU9" s="7"/>
+      <c r="AV9" s="7"/>
+      <c r="AW9" s="7"/>
+      <c r="AX9" s="7"/>
+      <c r="AY9" s="7"/>
+      <c r="AZ9" s="7"/>
+      <c r="BA9" s="7"/>
+      <c r="BB9" s="7"/>
+      <c r="BC9" s="7"/>
+      <c r="BF9" s="7"/>
+      <c r="BG9" s="7"/>
+      <c r="BH9" s="7"/>
+      <c r="BI9" s="7"/>
+      <c r="BJ9" s="7"/>
+      <c r="BM9" s="7"/>
+      <c r="BN9" s="7"/>
+      <c r="BO9" s="7"/>
+      <c r="BP9" s="7"/>
+      <c r="BQ9" s="7"/>
     </row>
-    <row r="10" spans="1:120" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:120" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="50"/>
+      <c r="F10" s="38"/>
     </row>
-    <row r="11" spans="1:120" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+    <row r="11" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="U11" s="37"/>
-      <c r="V11" s="37"/>
-      <c r="AB11" s="37"/>
-      <c r="AC11" s="37"/>
-      <c r="AI11" s="37"/>
-      <c r="AJ11" s="37"/>
-      <c r="AP11" s="37"/>
-      <c r="AQ11" s="37"/>
-      <c r="AW11" s="37"/>
-      <c r="AX11" s="37"/>
-      <c r="BD11" s="37"/>
-      <c r="BE11" s="37"/>
-      <c r="BK11" s="37"/>
-      <c r="BL11" s="37"/>
-      <c r="BR11" s="37"/>
-      <c r="BS11" s="37"/>
-      <c r="BY11" s="37"/>
-      <c r="BZ11" s="37"/>
-      <c r="CF11" s="37"/>
-      <c r="CG11" s="37"/>
-      <c r="CM11" s="37"/>
-      <c r="CN11" s="37"/>
-      <c r="CT11" s="37"/>
-      <c r="CU11" s="37"/>
-      <c r="DA11" s="37"/>
-      <c r="DB11" s="37"/>
-      <c r="DD11" s="22"/>
-      <c r="DE11" s="22"/>
-      <c r="DH11" s="37"/>
-      <c r="DI11" s="37"/>
-      <c r="DK11" s="23"/>
-      <c r="DO11" s="37"/>
-      <c r="DP11" s="37"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:120" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="U12" s="37"/>
-      <c r="V12" s="37"/>
-      <c r="AB12" s="37"/>
-      <c r="AC12" s="37"/>
-      <c r="AI12" s="37"/>
-      <c r="AJ12" s="37"/>
-      <c r="AP12" s="37"/>
-      <c r="AQ12" s="37"/>
-      <c r="AW12" s="37"/>
-      <c r="AX12" s="37"/>
-      <c r="BD12" s="37"/>
-      <c r="BE12" s="37"/>
-      <c r="BK12" s="37"/>
-      <c r="BL12" s="37"/>
-      <c r="BR12" s="37"/>
-      <c r="BS12" s="37"/>
-      <c r="BY12" s="37"/>
-      <c r="BZ12" s="37"/>
-      <c r="CF12" s="37"/>
-      <c r="CG12" s="37"/>
-      <c r="CM12" s="37"/>
-      <c r="CN12" s="37"/>
-      <c r="CT12" s="37"/>
-      <c r="CU12" s="37"/>
-      <c r="DA12" s="37"/>
-      <c r="DB12" s="37"/>
-      <c r="DD12" s="22"/>
-      <c r="DE12" s="22"/>
-      <c r="DH12" s="37"/>
-      <c r="DI12" s="37"/>
-      <c r="DK12" s="23"/>
-      <c r="DO12" s="37"/>
-      <c r="DP12" s="37"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
     </row>
-    <row r="13" spans="1:120" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+    <row r="13" spans="1:120" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="51"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="36"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="38"/>
-      <c r="X13" s="38"/>
-      <c r="Y13" s="38"/>
-      <c r="Z13" s="38"/>
-      <c r="AA13" s="38"/>
-      <c r="AB13" s="36"/>
-      <c r="AC13" s="36"/>
-      <c r="AD13" s="38"/>
-      <c r="AE13" s="38"/>
-      <c r="AF13" s="38"/>
-      <c r="AG13" s="38"/>
-      <c r="AH13" s="38"/>
-      <c r="AI13" s="36"/>
-      <c r="AJ13" s="36"/>
-      <c r="AP13" s="36"/>
-      <c r="AQ13" s="36"/>
-      <c r="AW13" s="36"/>
-      <c r="AX13" s="36"/>
-      <c r="BD13" s="36"/>
-      <c r="BE13" s="36"/>
-      <c r="BK13" s="36"/>
-      <c r="BL13" s="36"/>
-      <c r="BR13" s="36"/>
-      <c r="BS13" s="36"/>
-      <c r="BY13" s="36"/>
-      <c r="BZ13" s="36"/>
-      <c r="CF13" s="36"/>
-      <c r="CG13" s="36"/>
-      <c r="CM13" s="36"/>
-      <c r="CN13" s="36"/>
-      <c r="CT13" s="36"/>
-      <c r="CU13" s="36"/>
-      <c r="DA13" s="36"/>
-      <c r="DB13" s="36"/>
-      <c r="DD13" s="25"/>
-      <c r="DE13" s="25"/>
-      <c r="DH13" s="36"/>
-      <c r="DI13" s="36"/>
-      <c r="DK13" s="26"/>
-      <c r="DO13" s="36"/>
-      <c r="DP13" s="36"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="27"/>
+      <c r="AC13" s="27"/>
+      <c r="AD13" s="28"/>
+      <c r="AE13" s="28"/>
+      <c r="AF13" s="28"/>
+      <c r="AG13" s="28"/>
+      <c r="AH13" s="28"/>
+      <c r="AI13" s="27"/>
+      <c r="AJ13" s="27"/>
+      <c r="AP13" s="27"/>
+      <c r="AQ13" s="27"/>
+      <c r="AW13" s="27"/>
+      <c r="AX13" s="27"/>
+      <c r="BD13" s="27"/>
+      <c r="BE13" s="27"/>
+      <c r="BK13" s="27"/>
+      <c r="BL13" s="27"/>
+      <c r="BR13" s="27"/>
+      <c r="BS13" s="27"/>
+      <c r="BY13" s="27"/>
+      <c r="BZ13" s="27"/>
+      <c r="CF13" s="27"/>
+      <c r="CG13" s="27"/>
+      <c r="CM13" s="27"/>
+      <c r="CN13" s="27"/>
+      <c r="CT13" s="27"/>
+      <c r="CU13" s="27"/>
+      <c r="DA13" s="27"/>
+      <c r="DB13" s="27"/>
+      <c r="DD13" s="18"/>
+      <c r="DE13" s="18"/>
+      <c r="DH13" s="27"/>
+      <c r="DI13" s="27"/>
+      <c r="DK13" s="19"/>
+      <c r="DO13" s="27"/>
+      <c r="DP13" s="27"/>
     </row>
-    <row r="14" spans="1:120" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+    <row r="14" spans="1:120" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="51"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="U14" s="36"/>
-      <c r="V14" s="36"/>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="38"/>
-      <c r="AA14" s="38"/>
-      <c r="AB14" s="36"/>
-      <c r="AC14" s="36"/>
-      <c r="AD14" s="38"/>
-      <c r="AE14" s="38"/>
-      <c r="AF14" s="38"/>
-      <c r="AG14" s="38"/>
-      <c r="AH14" s="38"/>
-      <c r="AI14" s="36"/>
-      <c r="AJ14" s="36"/>
-      <c r="AP14" s="36"/>
-      <c r="AQ14" s="36"/>
-      <c r="AW14" s="36"/>
-      <c r="AX14" s="36"/>
-      <c r="BD14" s="36"/>
-      <c r="BE14" s="36"/>
-      <c r="BK14" s="36"/>
-      <c r="BL14" s="36"/>
-      <c r="BR14" s="36"/>
-      <c r="BS14" s="36"/>
-      <c r="BY14" s="36"/>
-      <c r="BZ14" s="36"/>
-      <c r="CF14" s="36"/>
-      <c r="CG14" s="36"/>
-      <c r="CM14" s="36"/>
-      <c r="CN14" s="36"/>
-      <c r="CT14" s="36"/>
-      <c r="CU14" s="36"/>
-      <c r="DA14" s="36"/>
-      <c r="DB14" s="36"/>
-      <c r="DD14" s="25"/>
-      <c r="DE14" s="25"/>
-      <c r="DH14" s="36"/>
-      <c r="DI14" s="36"/>
-      <c r="DK14" s="26"/>
-      <c r="DO14" s="36"/>
-      <c r="DP14" s="36"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="Y14" s="28"/>
+      <c r="Z14" s="28"/>
+      <c r="AA14" s="28"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="28"/>
+      <c r="AE14" s="28"/>
+      <c r="AF14" s="28"/>
+      <c r="AG14" s="28"/>
+      <c r="AH14" s="28"/>
+      <c r="AI14" s="27"/>
+      <c r="AJ14" s="27"/>
+      <c r="AP14" s="27"/>
+      <c r="AQ14" s="27"/>
+      <c r="AW14" s="27"/>
+      <c r="AX14" s="27"/>
+      <c r="BD14" s="27"/>
+      <c r="BE14" s="27"/>
+      <c r="BK14" s="27"/>
+      <c r="BL14" s="27"/>
+      <c r="BR14" s="27"/>
+      <c r="BS14" s="27"/>
+      <c r="BY14" s="27"/>
+      <c r="BZ14" s="27"/>
+      <c r="CF14" s="27"/>
+      <c r="CG14" s="27"/>
+      <c r="CM14" s="27"/>
+      <c r="CN14" s="27"/>
+      <c r="CT14" s="27"/>
+      <c r="CU14" s="27"/>
+      <c r="DA14" s="27"/>
+      <c r="DB14" s="27"/>
+      <c r="DD14" s="18"/>
+      <c r="DE14" s="18"/>
+      <c r="DH14" s="27"/>
+      <c r="DI14" s="27"/>
+      <c r="DK14" s="19"/>
+      <c r="DO14" s="27"/>
+      <c r="DP14" s="27"/>
     </row>
-    <row r="15" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+    <row r="15" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="AK15" s="39"/>
-      <c r="AL15" s="39"/>
-      <c r="AM15" s="39"/>
-      <c r="AN15" s="39"/>
-      <c r="AO15" s="39"/>
-      <c r="AR15" s="39"/>
-      <c r="AS15" s="39"/>
-      <c r="AT15" s="39"/>
-      <c r="AU15" s="39"/>
-      <c r="AV15" s="39"/>
+      <c r="AK15" s="22"/>
+      <c r="AL15" s="22"/>
+      <c r="AM15" s="22"/>
+      <c r="AN15" s="22"/>
+      <c r="AO15" s="22"/>
+      <c r="AR15" s="22"/>
+      <c r="AS15" s="22"/>
+      <c r="AT15" s="22"/>
+      <c r="AU15" s="22"/>
+      <c r="AV15" s="22"/>
     </row>
-    <row r="16" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+    <row r="16" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="W16" s="39"/>
-      <c r="X16" s="39"/>
-      <c r="Y16" s="39"/>
-      <c r="Z16" s="39"/>
-      <c r="AA16" s="39"/>
-      <c r="AD16" s="39"/>
-      <c r="AE16" s="39"/>
-      <c r="AF16" s="39"/>
-      <c r="AG16" s="39"/>
-      <c r="AH16" s="39"/>
-      <c r="AK16" s="39"/>
-      <c r="AL16" s="39"/>
-      <c r="AM16" s="39"/>
-      <c r="AN16" s="39"/>
-      <c r="AO16" s="39"/>
-      <c r="AR16" s="39"/>
-      <c r="AS16" s="39"/>
-      <c r="AT16" s="39"/>
-      <c r="AU16" s="39"/>
-      <c r="AV16" s="39"/>
-      <c r="AY16" s="39"/>
-      <c r="AZ16" s="39"/>
-      <c r="BA16" s="39"/>
-      <c r="BB16" s="39"/>
-      <c r="BC16" s="39"/>
+      <c r="W16" s="22"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="22"/>
+      <c r="AA16" s="22"/>
+      <c r="AD16" s="22"/>
+      <c r="AE16" s="22"/>
+      <c r="AF16" s="22"/>
+      <c r="AG16" s="22"/>
+      <c r="AH16" s="22"/>
+      <c r="AK16" s="22"/>
+      <c r="AL16" s="22"/>
+      <c r="AM16" s="22"/>
+      <c r="AN16" s="22"/>
+      <c r="AO16" s="22"/>
+      <c r="AR16" s="22"/>
+      <c r="AS16" s="22"/>
+      <c r="AT16" s="22"/>
+      <c r="AU16" s="22"/>
+      <c r="AV16" s="22"/>
+      <c r="AY16" s="22"/>
+      <c r="AZ16" s="22"/>
+      <c r="BA16" s="22"/>
+      <c r="BB16" s="22"/>
+      <c r="BC16" s="22"/>
     </row>
-    <row r="17" spans="1:6" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+    <row r="17" spans="1:83" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="50"/>
+      <c r="F17" s="38"/>
     </row>
-    <row r="24" spans="1:6" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+    <row r="24" spans="1:83" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="37"/>
+    </row>
+    <row r="25" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+    </row>
+    <row r="26" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+    </row>
+    <row r="27" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+    </row>
+    <row r="28" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22"/>
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="22"/>
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+      <c r="AD28" s="22"/>
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="22"/>
+      <c r="AH28" s="22"/>
+    </row>
+    <row r="29" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK29" s="22"/>
+      <c r="AL29" s="22"/>
+      <c r="AM29" s="22"/>
+      <c r="AN29" s="22"/>
+      <c r="AO29" s="22"/>
+    </row>
+    <row r="30" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR30" s="22"/>
+      <c r="AS30" s="22"/>
+      <c r="AT30" s="22"/>
+      <c r="AU30" s="22"/>
+      <c r="AV30" s="22"/>
+      <c r="AW30" s="22"/>
+      <c r="AX30" s="22"/>
+      <c r="AY30" s="22"/>
+      <c r="AZ30" s="22"/>
+      <c r="BA30" s="22"/>
+      <c r="BB30" s="22"/>
+      <c r="BC30" s="22"/>
+      <c r="BD30" s="22"/>
+      <c r="BE30" s="22"/>
+      <c r="BF30" s="22"/>
+      <c r="BG30" s="22"/>
+      <c r="BH30" s="22"/>
+      <c r="BI30" s="22"/>
+      <c r="BJ30" s="22"/>
+      <c r="BK30" s="22"/>
+      <c r="BL30" s="22"/>
+      <c r="BM30" s="22"/>
+      <c r="BN30" s="22"/>
+      <c r="BO30" s="22"/>
+      <c r="BP30" s="22"/>
+      <c r="BQ30" s="22"/>
+      <c r="BR30" s="22"/>
+      <c r="BS30" s="22"/>
+      <c r="BT30" s="22"/>
+      <c r="BU30" s="22"/>
+      <c r="BV30" s="22"/>
+      <c r="BW30" s="22"/>
+      <c r="BX30" s="22"/>
+      <c r="BY30" s="22"/>
+      <c r="BZ30" s="22"/>
+      <c r="CA30" s="22"/>
+      <c r="CB30" s="22"/>
+      <c r="CC30" s="22"/>
+      <c r="CD30" s="22"/>
+      <c r="CE30" s="22"/>
+    </row>
+    <row r="31" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
+      <c r="T31" s="43"/>
+      <c r="U31" s="43"/>
+      <c r="V31" s="43"/>
+      <c r="W31" s="43"/>
+      <c r="X31" s="43"/>
+      <c r="Y31" s="43"/>
+      <c r="Z31" s="43"/>
+      <c r="AA31" s="43"/>
+      <c r="AB31" s="43"/>
+      <c r="AC31" s="43"/>
+      <c r="AD31" s="43"/>
+      <c r="AE31" s="43"/>
+      <c r="AF31" s="43"/>
+      <c r="AG31" s="43"/>
+      <c r="AH31" s="43"/>
+      <c r="AI31" s="43"/>
+      <c r="AJ31" s="43"/>
+      <c r="AK31" s="43"/>
+      <c r="AL31" s="43"/>
+      <c r="AM31" s="43"/>
+      <c r="AN31" s="43"/>
+      <c r="AO31" s="43"/>
+      <c r="AP31" s="43"/>
+      <c r="AQ31" s="43"/>
+      <c r="AR31" s="43"/>
+      <c r="AS31" s="43"/>
+      <c r="AT31" s="43"/>
+      <c r="AU31" s="43"/>
+      <c r="AV31" s="43"/>
+      <c r="AW31" s="43"/>
+      <c r="AX31" s="43"/>
+      <c r="AY31" s="43"/>
+      <c r="AZ31" s="43"/>
+      <c r="BA31" s="43"/>
+      <c r="BB31" s="43"/>
+      <c r="BC31" s="43"/>
+      <c r="BD31" s="43"/>
+      <c r="BE31" s="43"/>
+      <c r="BF31" s="43"/>
+      <c r="BG31" s="43"/>
+      <c r="BH31" s="43"/>
+      <c r="BI31" s="43"/>
+      <c r="BJ31" s="43"/>
+      <c r="BK31" s="43"/>
+      <c r="BL31" s="43"/>
+      <c r="BM31" s="43"/>
+      <c r="BN31" s="43"/>
+      <c r="BO31" s="43"/>
+      <c r="BP31" s="43"/>
+      <c r="BQ31" s="43"/>
+      <c r="BR31" s="43"/>
+      <c r="BS31" s="43"/>
+      <c r="BT31" s="43"/>
+      <c r="BU31" s="43"/>
+      <c r="BV31" s="43"/>
+      <c r="BW31" s="43"/>
+      <c r="BX31" s="43"/>
+      <c r="BY31" s="43"/>
+      <c r="BZ31" s="43"/>
+      <c r="CA31" s="43"/>
+      <c r="CB31" s="43"/>
+      <c r="CC31" s="43"/>
+      <c r="CD31" s="43"/>
+      <c r="CE31" s="43"/>
+    </row>
+    <row r="32" spans="1:83" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="49"/>
-    </row>
-    <row r="31" spans="1:6" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="50"/>
+      <c r="F32" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="I4:O4"/>
@@ -3340,6 +3443,16 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.78740157480314965" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3351,27 +3464,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0">0-93518095-55993</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0">
-      <Url>https://evonik.sharepoint.com/sites/13129/_layouts/15/DocIdRedir.aspx?ID=0-93518095-55993</Url>
-      <Description>0-93518095-55993</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D98DF252718B14F9C13E50871EB3D76" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="33c83fdbb9e9dd0c2649960876b7423f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0" xmlns:ns3="909da4c9-3531-4fb4-a16c-fe746456455a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ab13681565d5f0eb6f0b0e10da5abf3" ns2:_="" ns3:_="">
     <xsd:import namespace="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0"/>
@@ -3599,6 +3691,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0">0-93518095-55993</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0">
+      <Url>https://evonik.sharepoint.com/sites/13129/_layouts/15/DocIdRedir.aspx?ID=0-93518095-55993</Url>
+      <Description>0-93518095-55993</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -3650,24 +3763,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1376E91E-7564-4EA7-82E9-F45D5BE229A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC31D3A6-4EB4-4E27-A5DB-8C0892094121}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6ACD257-8FA8-4D4D-8960-D1074C7DEC25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3686,6 +3781,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC31D3A6-4EB4-4E27-A5DB-8C0892094121}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1376E91E-7564-4EA7-82E9-F45D5BE229A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E01570BF-52F9-46B8-9C85-26D2F1ECBEF4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
upload final gantt chart
</commit_message>
<xml_diff>
--- a/docs/gantt_chart_secrecy.xlsx
+++ b/docs/gantt_chart_secrecy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mimoun.mendoughe/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D23031\OneDrive - Evonik Industries AG\Dokumente\personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE6CE7D-10DB-7145-9EF1-483A4AF486A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF1F255-7D06-4883-B0B4-6AAA210D61AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30940" windowHeight="16780" xr2:uid="{D30480B8-D58C-44F1-852C-2B52D77C9917}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D30480B8-D58C-44F1-852C-2B52D77C9917}"/>
   </bookViews>
   <sheets>
     <sheet name="Mappe 1" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="55">
   <si>
     <t>FESCA Project</t>
   </si>
@@ -76,9 +76,6 @@
     <t>KW 30</t>
   </si>
   <si>
-    <t>KW 24</t>
-  </si>
-  <si>
     <t>KW 25</t>
   </si>
   <si>
@@ -118,58 +115,97 @@
     <t>KW 40</t>
   </si>
   <si>
-    <t>1a SQL Parsing</t>
-  </si>
-  <si>
     <t>1b Logical Plan construction</t>
   </si>
   <si>
-    <t>1c Secrecy aligned MPC-aware cost model</t>
-  </si>
-  <si>
-    <t>1 SQL Query Engine (Darya)</t>
-  </si>
-  <si>
-    <t>1d Query optimization</t>
-  </si>
-  <si>
-    <t>1e Physical Plan generation</t>
-  </si>
-  <si>
-    <t>1f Integration and testing</t>
-  </si>
-  <si>
-    <t>2 MPC Runtime and oblivious operators</t>
-  </si>
-  <si>
-    <t>4 MPC Protocol layer</t>
-  </si>
-  <si>
     <t>KW 27 (June-July)</t>
   </si>
   <si>
-    <t>3a Interface for Uploading tables</t>
-  </si>
-  <si>
     <t>3b Row Reader &amp; Bit String Encoder</t>
   </si>
   <si>
-    <t>3c Generating shares for tuple</t>
-  </si>
-  <si>
     <t>3d Generating shares of a table</t>
   </si>
   <si>
-    <t>3e Setting up the receive procedure</t>
-  </si>
-  <si>
-    <t>3 Secret Sharing and data ingestion (Mimoun)</t>
-  </si>
-  <si>
-    <t>3f Integration</t>
-  </si>
-  <si>
-    <t>3g testing</t>
+    <t>Crypto Layer</t>
+  </si>
+  <si>
+    <t>Communication Layer</t>
+  </si>
+  <si>
+    <t>1c Physical Plan generation</t>
+  </si>
+  <si>
+    <t>1a SQL Parsing (Query-AST)</t>
+  </si>
+  <si>
+    <t>gRPC send result to analyst after computation</t>
+  </si>
+  <si>
+    <t>gRPC communication for MPC primitives</t>
+  </si>
+  <si>
+    <t>3a Interface for Uploading tables (maybe application layer?)</t>
+  </si>
+  <si>
+    <t>1d physical plan &lt;-&gt; MPC circuit translation, attention to and and xor</t>
+  </si>
+  <si>
+    <t>Application Layer (Darya)</t>
+  </si>
+  <si>
+    <t>Computing nodes</t>
+  </si>
+  <si>
+    <t>3c Generating shares for tuple (implies generating randomness)</t>
+  </si>
+  <si>
+    <t>Composition execution (layer by layer)</t>
+  </si>
+  <si>
+    <t>Apply vectorizing (?)</t>
+  </si>
+  <si>
+    <t>gRPC send shares of tables to comp. nodes</t>
+  </si>
+  <si>
+    <t>(from 1d) gRPC submit query as a circuit, maybe add. Info to all nodes, returns ack</t>
+  </si>
+  <si>
+    <t>Receive results from nodes, Reconstruct computation results</t>
+  </si>
+  <si>
+    <t>Entities:</t>
+  </si>
+  <si>
+    <t>Unit tests</t>
+  </si>
+  <si>
+    <t>Latency test: Small dataset</t>
+  </si>
+  <si>
+    <t>Latency test: Large dataset</t>
+  </si>
+  <si>
+    <t>Dockerize all entities / evaluation / wrapping up</t>
+  </si>
+  <si>
+    <t>Data Owner (Mimoun)</t>
+  </si>
+  <si>
+    <t>Data Analyst (Darya)</t>
+  </si>
+  <si>
+    <t>Generate correlated randomness (Alisher, Denis)</t>
+  </si>
+  <si>
+    <t>XOR gate execution (Alisher, Denis)</t>
+  </si>
+  <si>
+    <t>AND gate execution (implies gRPC) (Alisher, Denis)</t>
+  </si>
+  <si>
+    <t>setup docker configuration file for all entities (Mimoun)</t>
   </si>
 </sst>
 </file>
@@ -177,12 +213,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;€&quot;* #,##0.00_);_(&quot;€&quot;* \(#,##0.00\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;€&quot;* #,##0.00_);_(&quot;€&quot;* \(#,##0.00\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,8 +377,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,25 +488,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,6 +496,42 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCECFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -586,23 +649,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -610,10 +673,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -625,10 +688,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -640,10 +703,10 @@
   </borders>
   <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
@@ -673,7 +736,7 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -711,52 +774,36 @@
     <xf numFmtId="0" fontId="19" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -767,7 +814,21 @@
     <xf numFmtId="0" fontId="17" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Accent1" xfId="22" builtinId="29" customBuiltin="1"/>
@@ -1621,8 +1682,13 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF99CCFF"/>
       <color rgb="FFFF5050"/>
-      <color rgb="FF99CCFF"/>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFCCECFF"/>
+      <color rgb="FFCCFF99"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFFF9966"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2035,622 +2101,589 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:DP32"/>
+  <dimension ref="A1:DI42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BB21" sqref="BB21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="7.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="1.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="37" max="41" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="44" max="48" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="51" max="54" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="1.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="1.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="65" max="69" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="72" max="76" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="77" max="78" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="79" max="83" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="84" max="85" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="89" max="90" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="91" max="92" width="1.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="95" max="97" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="98" max="99" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="100" max="104" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="105" max="106" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="108" max="109" width="1.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="110" max="111" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="112" max="113" width="1.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="1.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="117" max="118" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="119" max="120" width="1.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.1796875" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="1.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="1.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="34" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="37" max="41" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="44" max="47" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="1.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="1.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="1.453125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="1.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="58" max="62" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="65" max="69" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="72" max="76" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="1.453125" bestFit="1" customWidth="1"/>
+    <col min="84" max="85" width="1.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="88" max="90" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="91" max="92" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="93" max="97" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="98" max="99" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="101" max="102" width="2.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="103" max="104" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="105" max="106" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="2.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="1.453125" bestFit="1" customWidth="1"/>
+    <col min="112" max="113" width="1.54296875" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="F1" s="33"/>
+      <c r="C1" s="22"/>
+      <c r="CW1"/>
+      <c r="CX1"/>
       <c r="DD1"/>
-      <c r="DE1"/>
-      <c r="DK1"/>
-    </row>
-    <row r="2" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+    </row>
+    <row r="2" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="CW2"/>
+      <c r="CX2"/>
       <c r="DD2"/>
-      <c r="DE2"/>
-      <c r="DK2"/>
-    </row>
-    <row r="3" spans="1:120" ht="19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:113" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="CW3"/>
+      <c r="CX3"/>
       <c r="DD3"/>
-      <c r="DE3"/>
-      <c r="DK3"/>
-    </row>
-    <row r="4" spans="1:120" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:113" ht="29.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="40" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="40" t="s">
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="X4" s="41"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="41"/>
-      <c r="AA4" s="41"/>
-      <c r="AB4" s="41"/>
-      <c r="AC4" s="42"/>
-      <c r="AD4" s="40" t="s">
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="32"/>
+      <c r="AD4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="AE4" s="41"/>
-      <c r="AF4" s="41"/>
-      <c r="AG4" s="41"/>
-      <c r="AH4" s="41"/>
-      <c r="AI4" s="41"/>
-      <c r="AJ4" s="42"/>
-      <c r="AK4" s="40" t="s">
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="31"/>
+      <c r="AG4" s="31"/>
+      <c r="AH4" s="31"/>
+      <c r="AI4" s="31"/>
+      <c r="AJ4" s="32"/>
+      <c r="AK4" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL4" s="31"/>
+      <c r="AM4" s="31"/>
+      <c r="AN4" s="31"/>
+      <c r="AO4" s="31"/>
+      <c r="AP4" s="31"/>
+      <c r="AQ4" s="32"/>
+      <c r="AR4" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS4" s="31"/>
+      <c r="AT4" s="31"/>
+      <c r="AU4" s="31"/>
+      <c r="AV4" s="31"/>
+      <c r="AW4" s="31"/>
+      <c r="AX4" s="32"/>
+      <c r="AY4" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ4" s="31"/>
+      <c r="BA4" s="31"/>
+      <c r="BB4" s="31"/>
+      <c r="BC4" s="31"/>
+      <c r="BD4" s="31"/>
+      <c r="BE4" s="32"/>
+      <c r="BF4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="AL4" s="41"/>
-      <c r="AM4" s="41"/>
-      <c r="AN4" s="41"/>
-      <c r="AO4" s="41"/>
-      <c r="AP4" s="41"/>
-      <c r="AQ4" s="42"/>
-      <c r="AR4" s="40" t="s">
+      <c r="BG4" s="31"/>
+      <c r="BH4" s="31"/>
+      <c r="BI4" s="31"/>
+      <c r="BJ4" s="31"/>
+      <c r="BK4" s="31"/>
+      <c r="BL4" s="32"/>
+      <c r="BM4" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="BN4" s="31"/>
+      <c r="BO4" s="31"/>
+      <c r="BP4" s="31"/>
+      <c r="BQ4" s="31"/>
+      <c r="BR4" s="31"/>
+      <c r="BS4" s="32"/>
+      <c r="BT4" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="BU4" s="31"/>
+      <c r="BV4" s="31"/>
+      <c r="BW4" s="31"/>
+      <c r="BX4" s="31"/>
+      <c r="BY4" s="31"/>
+      <c r="BZ4" s="32"/>
+      <c r="CA4" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="CB4" s="31"/>
+      <c r="CC4" s="31"/>
+      <c r="CD4" s="31"/>
+      <c r="CE4" s="31"/>
+      <c r="CF4" s="31"/>
+      <c r="CG4" s="32"/>
+      <c r="CH4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="CI4" s="31"/>
+      <c r="CJ4" s="31"/>
+      <c r="CK4" s="31"/>
+      <c r="CL4" s="31"/>
+      <c r="CM4" s="31"/>
+      <c r="CN4" s="32"/>
+      <c r="CO4" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="CP4" s="31"/>
+      <c r="CQ4" s="31"/>
+      <c r="CR4" s="31"/>
+      <c r="CS4" s="31"/>
+      <c r="CT4" s="31"/>
+      <c r="CU4" s="32"/>
+      <c r="CV4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="CW4" s="31"/>
+      <c r="CX4" s="31"/>
+      <c r="CY4" s="31"/>
+      <c r="CZ4" s="31"/>
+      <c r="DA4" s="31"/>
+      <c r="DB4" s="32"/>
+      <c r="DC4" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="DD4" s="31"/>
+      <c r="DE4" s="31"/>
+      <c r="DF4" s="31"/>
+      <c r="DG4" s="31"/>
+      <c r="DH4" s="31"/>
+      <c r="DI4" s="32"/>
+    </row>
+    <row r="5" spans="1:113" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3">
+        <v>16</v>
+      </c>
+      <c r="C5" s="24">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2">
+        <v>20</v>
+      </c>
+      <c r="G5" s="17">
+        <v>21</v>
+      </c>
+      <c r="H5" s="18">
+        <v>22</v>
+      </c>
+      <c r="I5" s="3">
+        <v>23</v>
+      </c>
+      <c r="J5" s="2">
+        <v>24</v>
+      </c>
+      <c r="K5" s="2">
+        <v>25</v>
+      </c>
+      <c r="L5" s="2">
+        <v>26</v>
+      </c>
+      <c r="M5" s="2">
+        <v>27</v>
+      </c>
+      <c r="N5" s="17">
+        <v>28</v>
+      </c>
+      <c r="O5" s="18">
+        <v>29</v>
+      </c>
+      <c r="P5" s="3">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>1</v>
+      </c>
+      <c r="R5" s="2">
+        <v>2</v>
+      </c>
+      <c r="S5" s="2">
+        <v>3</v>
+      </c>
+      <c r="T5" s="2">
+        <v>4</v>
+      </c>
+      <c r="U5" s="17">
+        <v>5</v>
+      </c>
+      <c r="V5" s="18">
+        <v>6</v>
+      </c>
+      <c r="W5" s="3">
+        <v>7</v>
+      </c>
+      <c r="X5" s="2">
+        <v>8</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="2">
         <v>10</v>
       </c>
-      <c r="AS4" s="41"/>
-      <c r="AT4" s="41"/>
-      <c r="AU4" s="41"/>
-      <c r="AV4" s="41"/>
-      <c r="AW4" s="41"/>
-      <c r="AX4" s="42"/>
-      <c r="AY4" s="40" t="s">
+      <c r="AA5" s="2">
+        <v>11</v>
+      </c>
+      <c r="AB5" s="17">
+        <v>12</v>
+      </c>
+      <c r="AC5" s="18">
+        <v>13</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>14</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>15</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>16</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>17</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>18</v>
+      </c>
+      <c r="AI5" s="17">
+        <v>19</v>
+      </c>
+      <c r="AJ5" s="18">
         <v>20</v>
       </c>
-      <c r="AZ4" s="41"/>
-      <c r="BA4" s="41"/>
-      <c r="BB4" s="41"/>
-      <c r="BC4" s="41"/>
-      <c r="BD4" s="41"/>
-      <c r="BE4" s="42"/>
-      <c r="BF4" s="40" t="s">
+      <c r="AK5" s="3">
+        <v>21</v>
+      </c>
+      <c r="AL5" s="2">
+        <v>22</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>23</v>
+      </c>
+      <c r="AN5" s="2">
+        <v>24</v>
+      </c>
+      <c r="AO5" s="2">
+        <v>25</v>
+      </c>
+      <c r="AP5" s="17">
+        <v>26</v>
+      </c>
+      <c r="AQ5" s="18">
+        <v>27</v>
+      </c>
+      <c r="AR5" s="3">
+        <v>28</v>
+      </c>
+      <c r="AS5" s="2">
+        <v>29</v>
+      </c>
+      <c r="AT5" s="2">
+        <v>30</v>
+      </c>
+      <c r="AU5" s="2">
+        <v>31</v>
+      </c>
+      <c r="AV5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="17">
+        <v>2</v>
+      </c>
+      <c r="AX5" s="17">
+        <v>3</v>
+      </c>
+      <c r="AY5" s="2">
+        <v>4</v>
+      </c>
+      <c r="AZ5" s="2">
+        <v>5</v>
+      </c>
+      <c r="BA5" s="2">
+        <v>6</v>
+      </c>
+      <c r="BB5" s="2">
+        <v>7</v>
+      </c>
+      <c r="BC5" s="2">
+        <v>8</v>
+      </c>
+      <c r="BD5" s="17">
         <v>9</v>
       </c>
-      <c r="BG4" s="41"/>
-      <c r="BH4" s="41"/>
-      <c r="BI4" s="41"/>
-      <c r="BJ4" s="41"/>
-      <c r="BK4" s="41"/>
-      <c r="BL4" s="42"/>
-      <c r="BM4" s="40" t="s">
+      <c r="BE5" s="17">
+        <v>10</v>
+      </c>
+      <c r="BF5" s="2">
+        <v>11</v>
+      </c>
+      <c r="BG5" s="2">
+        <v>12</v>
+      </c>
+      <c r="BH5" s="2">
+        <v>13</v>
+      </c>
+      <c r="BI5" s="2">
+        <v>14</v>
+      </c>
+      <c r="BJ5" s="2">
+        <v>15</v>
+      </c>
+      <c r="BK5" s="17">
         <v>16</v>
       </c>
-      <c r="BN4" s="41"/>
-      <c r="BO4" s="41"/>
-      <c r="BP4" s="41"/>
-      <c r="BQ4" s="41"/>
-      <c r="BR4" s="41"/>
-      <c r="BS4" s="42"/>
-      <c r="BT4" s="40" t="s">
+      <c r="BL5" s="17">
         <v>17</v>
       </c>
-      <c r="BU4" s="41"/>
-      <c r="BV4" s="41"/>
-      <c r="BW4" s="41"/>
-      <c r="BX4" s="41"/>
-      <c r="BY4" s="41"/>
-      <c r="BZ4" s="42"/>
-      <c r="CA4" s="40" t="s">
+      <c r="BM5" s="2">
         <v>18</v>
       </c>
-      <c r="CB4" s="41"/>
-      <c r="CC4" s="41"/>
-      <c r="CD4" s="41"/>
-      <c r="CE4" s="41"/>
-      <c r="CF4" s="41"/>
-      <c r="CG4" s="42"/>
-      <c r="CH4" s="40" t="s">
+      <c r="BN5" s="2">
         <v>19</v>
       </c>
-      <c r="CI4" s="41"/>
-      <c r="CJ4" s="41"/>
-      <c r="CK4" s="41"/>
-      <c r="CL4" s="41"/>
-      <c r="CM4" s="41"/>
-      <c r="CN4" s="42"/>
-      <c r="CO4" s="40" t="s">
+      <c r="BO5" s="2">
+        <v>20</v>
+      </c>
+      <c r="BP5" s="2">
         <v>21</v>
       </c>
-      <c r="CP4" s="41"/>
-      <c r="CQ4" s="41"/>
-      <c r="CR4" s="41"/>
-      <c r="CS4" s="41"/>
-      <c r="CT4" s="41"/>
-      <c r="CU4" s="42"/>
-      <c r="CV4" s="40" t="s">
+      <c r="BQ5" s="2">
         <v>22</v>
       </c>
-      <c r="CW4" s="41"/>
-      <c r="CX4" s="41"/>
-      <c r="CY4" s="41"/>
-      <c r="CZ4" s="41"/>
-      <c r="DA4" s="41"/>
-      <c r="DB4" s="42"/>
-      <c r="DC4" s="40" t="s">
+      <c r="BR5" s="17">
         <v>23</v>
       </c>
-      <c r="DD4" s="41"/>
-      <c r="DE4" s="41"/>
-      <c r="DF4" s="41"/>
-      <c r="DG4" s="41"/>
-      <c r="DH4" s="41"/>
-      <c r="DI4" s="42"/>
-      <c r="DJ4" s="40" t="s">
+      <c r="BS5" s="17">
         <v>24</v>
       </c>
-      <c r="DK4" s="41"/>
-      <c r="DL4" s="41"/>
-      <c r="DM4" s="41"/>
-      <c r="DN4" s="41"/>
-      <c r="DO4" s="41"/>
-      <c r="DP4" s="42"/>
-    </row>
-    <row r="5" spans="1:120" ht="19" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2">
+      <c r="BT5" s="2">
+        <v>25</v>
+      </c>
+      <c r="BU5" s="2">
+        <v>26</v>
+      </c>
+      <c r="BV5" s="2">
+        <v>27</v>
+      </c>
+      <c r="BW5" s="2">
+        <v>28</v>
+      </c>
+      <c r="BX5" s="2">
+        <v>29</v>
+      </c>
+      <c r="BY5" s="17">
+        <v>30</v>
+      </c>
+      <c r="BZ5" s="17">
+        <v>31</v>
+      </c>
+      <c r="CA5" s="8">
+        <v>1</v>
+      </c>
+      <c r="CB5" s="8">
+        <v>2</v>
+      </c>
+      <c r="CC5" s="8">
+        <v>3</v>
+      </c>
+      <c r="CD5" s="8">
+        <v>4</v>
+      </c>
+      <c r="CE5" s="8">
+        <v>5</v>
+      </c>
+      <c r="CF5" s="21">
+        <v>6</v>
+      </c>
+      <c r="CG5" s="21">
+        <v>7</v>
+      </c>
+      <c r="CH5" s="8">
+        <v>8</v>
+      </c>
+      <c r="CI5" s="8">
         <v>9</v>
       </c>
-      <c r="C5" s="2">
+      <c r="CJ5" s="8">
         <v>10</v>
       </c>
-      <c r="D5" s="2">
+      <c r="CK5" s="8">
         <v>11</v>
       </c>
-      <c r="E5" s="2">
+      <c r="CL5" s="8">
         <v>12</v>
       </c>
-      <c r="F5" s="35">
+      <c r="CM5" s="21">
         <v>13</v>
       </c>
-      <c r="G5" s="24">
+      <c r="CN5" s="21">
         <v>14</v>
       </c>
-      <c r="H5" s="25">
+      <c r="CO5" s="8">
         <v>15</v>
       </c>
-      <c r="I5" s="3">
+      <c r="CP5" s="8">
         <v>16</v>
       </c>
-      <c r="J5" s="2">
+      <c r="CQ5" s="8">
         <v>17</v>
       </c>
-      <c r="K5" s="2">
+      <c r="CR5" s="8">
         <v>18</v>
       </c>
-      <c r="L5" s="2">
+      <c r="CS5" s="8">
         <v>19</v>
       </c>
-      <c r="M5" s="2">
+      <c r="CT5" s="21">
         <v>20</v>
       </c>
-      <c r="N5" s="24">
+      <c r="CU5" s="21">
         <v>21</v>
       </c>
-      <c r="O5" s="25">
+      <c r="CV5" s="8">
         <v>22</v>
       </c>
-      <c r="P5" s="3">
+      <c r="CW5" s="13">
         <v>23</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="CX5" s="13">
         <v>24</v>
       </c>
-      <c r="R5" s="2">
+      <c r="CY5" s="8">
         <v>25</v>
       </c>
-      <c r="S5" s="2">
+      <c r="CZ5" s="8">
         <v>26</v>
       </c>
-      <c r="T5" s="2">
+      <c r="DA5" s="21">
         <v>27</v>
       </c>
-      <c r="U5" s="24">
+      <c r="DB5" s="21">
         <v>28</v>
       </c>
-      <c r="V5" s="25">
+      <c r="DC5" s="8">
         <v>29</v>
       </c>
-      <c r="W5" s="3">
+      <c r="DD5" s="10">
         <v>30</v>
       </c>
-      <c r="X5" s="2">
+    </row>
+    <row r="6" spans="1:113" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="C6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="E6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AB5" s="24">
+      <c r="G6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AC5" s="25">
-        <v>6</v>
-      </c>
-      <c r="AD5" s="3">
-        <v>7</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>8</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>9</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AH5" s="2">
-        <v>11</v>
-      </c>
-      <c r="AI5" s="24">
-        <v>12</v>
-      </c>
-      <c r="AJ5" s="25">
-        <v>13</v>
-      </c>
-      <c r="AK5" s="3">
-        <v>14</v>
-      </c>
-      <c r="AL5" s="2">
-        <v>15</v>
-      </c>
-      <c r="AM5" s="2">
-        <v>16</v>
-      </c>
-      <c r="AN5" s="2">
-        <v>17</v>
-      </c>
-      <c r="AO5" s="2">
-        <v>18</v>
-      </c>
-      <c r="AP5" s="24">
-        <v>19</v>
-      </c>
-      <c r="AQ5" s="25">
-        <v>20</v>
-      </c>
-      <c r="AR5" s="3">
-        <v>21</v>
-      </c>
-      <c r="AS5" s="2">
-        <v>22</v>
-      </c>
-      <c r="AT5" s="2">
-        <v>23</v>
-      </c>
-      <c r="AU5" s="2">
-        <v>24</v>
-      </c>
-      <c r="AV5" s="2">
-        <v>25</v>
-      </c>
-      <c r="AW5" s="24">
-        <v>26</v>
-      </c>
-      <c r="AX5" s="25">
-        <v>27</v>
-      </c>
-      <c r="AY5" s="3">
-        <v>28</v>
-      </c>
-      <c r="AZ5" s="2">
-        <v>29</v>
-      </c>
-      <c r="BA5" s="2">
-        <v>30</v>
-      </c>
-      <c r="BB5" s="2">
-        <v>31</v>
-      </c>
-      <c r="BC5" s="2">
-        <v>1</v>
-      </c>
-      <c r="BD5" s="24">
-        <v>2</v>
-      </c>
-      <c r="BE5" s="24">
-        <v>3</v>
-      </c>
-      <c r="BF5" s="2">
-        <v>4</v>
-      </c>
-      <c r="BG5" s="2">
-        <v>5</v>
-      </c>
-      <c r="BH5" s="2">
-        <v>6</v>
-      </c>
-      <c r="BI5" s="2">
-        <v>7</v>
-      </c>
-      <c r="BJ5" s="2">
-        <v>8</v>
-      </c>
-      <c r="BK5" s="24">
-        <v>9</v>
-      </c>
-      <c r="BL5" s="24">
-        <v>10</v>
-      </c>
-      <c r="BM5" s="2">
-        <v>11</v>
-      </c>
-      <c r="BN5" s="2">
-        <v>12</v>
-      </c>
-      <c r="BO5" s="2">
-        <v>13</v>
-      </c>
-      <c r="BP5" s="2">
-        <v>14</v>
-      </c>
-      <c r="BQ5" s="2">
-        <v>15</v>
-      </c>
-      <c r="BR5" s="24">
-        <v>16</v>
-      </c>
-      <c r="BS5" s="24">
-        <v>17</v>
-      </c>
-      <c r="BT5" s="2">
-        <v>18</v>
-      </c>
-      <c r="BU5" s="2">
-        <v>19</v>
-      </c>
-      <c r="BV5" s="2">
-        <v>20</v>
-      </c>
-      <c r="BW5" s="2">
-        <v>21</v>
-      </c>
-      <c r="BX5" s="2">
-        <v>22</v>
-      </c>
-      <c r="BY5" s="24">
-        <v>23</v>
-      </c>
-      <c r="BZ5" s="24">
-        <v>24</v>
-      </c>
-      <c r="CA5" s="2">
-        <v>25</v>
-      </c>
-      <c r="CB5" s="2">
-        <v>26</v>
-      </c>
-      <c r="CC5" s="2">
-        <v>27</v>
-      </c>
-      <c r="CD5" s="2">
-        <v>28</v>
-      </c>
-      <c r="CE5" s="2">
-        <v>29</v>
-      </c>
-      <c r="CF5" s="24">
-        <v>30</v>
-      </c>
-      <c r="CG5" s="24">
-        <v>31</v>
-      </c>
-      <c r="CH5" s="8">
-        <v>1</v>
-      </c>
-      <c r="CI5" s="8">
-        <v>2</v>
-      </c>
-      <c r="CJ5" s="8">
-        <v>3</v>
-      </c>
-      <c r="CK5" s="8">
-        <v>4</v>
-      </c>
-      <c r="CL5" s="8">
-        <v>5</v>
-      </c>
-      <c r="CM5" s="30">
-        <v>6</v>
-      </c>
-      <c r="CN5" s="30">
-        <v>7</v>
-      </c>
-      <c r="CO5" s="8">
-        <v>8</v>
-      </c>
-      <c r="CP5" s="8">
-        <v>9</v>
-      </c>
-      <c r="CQ5" s="8">
-        <v>10</v>
-      </c>
-      <c r="CR5" s="8">
-        <v>11</v>
-      </c>
-      <c r="CS5" s="8">
-        <v>12</v>
-      </c>
-      <c r="CT5" s="30">
-        <v>13</v>
-      </c>
-      <c r="CU5" s="30">
-        <v>14</v>
-      </c>
-      <c r="CV5" s="8">
-        <v>15</v>
-      </c>
-      <c r="CW5" s="8">
-        <v>16</v>
-      </c>
-      <c r="CX5" s="8">
-        <v>17</v>
-      </c>
-      <c r="CY5" s="8">
-        <v>18</v>
-      </c>
-      <c r="CZ5" s="8">
-        <v>19</v>
-      </c>
-      <c r="DA5" s="30">
-        <v>20</v>
-      </c>
-      <c r="DB5" s="30">
-        <v>21</v>
-      </c>
-      <c r="DC5" s="8">
-        <v>22</v>
-      </c>
-      <c r="DD5" s="13">
-        <v>23</v>
-      </c>
-      <c r="DE5" s="13">
-        <v>24</v>
-      </c>
-      <c r="DF5" s="8">
-        <v>25</v>
-      </c>
-      <c r="DG5" s="8">
-        <v>26</v>
-      </c>
-      <c r="DH5" s="30">
-        <v>27</v>
-      </c>
-      <c r="DI5" s="30">
-        <v>28</v>
-      </c>
-      <c r="DJ5" s="8">
-        <v>29</v>
-      </c>
-      <c r="DK5" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:120" ht="19" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="19" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="5" t="s">
@@ -2668,10 +2701,10 @@
       <c r="M6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="26" t="s">
+      <c r="N6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="26" t="s">
+      <c r="O6" s="19" t="s">
         <v>5</v>
       </c>
       <c r="P6" s="5" t="s">
@@ -2689,10 +2722,10 @@
       <c r="T6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="U6" s="26" t="s">
+      <c r="U6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="V6" s="26" t="s">
+      <c r="V6" s="19" t="s">
         <v>5</v>
       </c>
       <c r="W6" s="5" t="s">
@@ -2710,10 +2743,10 @@
       <c r="AA6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AB6" s="26" t="s">
+      <c r="AB6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AC6" s="26" t="s">
+      <c r="AC6" s="19" t="s">
         <v>5</v>
       </c>
       <c r="AD6" s="5" t="s">
@@ -2731,10 +2764,10 @@
       <c r="AH6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AI6" s="26" t="s">
+      <c r="AI6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AJ6" s="26" t="s">
+      <c r="AJ6" s="19" t="s">
         <v>5</v>
       </c>
       <c r="AK6" s="5" t="s">
@@ -2752,10 +2785,10 @@
       <c r="AO6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AP6" s="26" t="s">
+      <c r="AP6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AQ6" s="26" t="s">
+      <c r="AQ6" s="19" t="s">
         <v>5</v>
       </c>
       <c r="AR6" s="5" t="s">
@@ -2773,10 +2806,10 @@
       <c r="AV6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AW6" s="26" t="s">
+      <c r="AW6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AX6" s="26" t="s">
+      <c r="AX6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="AY6" s="5" t="s">
@@ -2794,10 +2827,10 @@
       <c r="BC6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BD6" s="26" t="s">
+      <c r="BD6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="BE6" s="29" t="s">
+      <c r="BE6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="BF6" s="5" t="s">
@@ -2815,10 +2848,10 @@
       <c r="BJ6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BK6" s="26" t="s">
+      <c r="BK6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="BL6" s="29" t="s">
+      <c r="BL6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="BM6" s="5" t="s">
@@ -2836,10 +2869,10 @@
       <c r="BQ6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BR6" s="26" t="s">
+      <c r="BR6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="BS6" s="29" t="s">
+      <c r="BS6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="BT6" s="5" t="s">
@@ -2857,10 +2890,10 @@
       <c r="BX6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BY6" s="26" t="s">
+      <c r="BY6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="BZ6" s="29" t="s">
+      <c r="BZ6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="CA6" s="5" t="s">
@@ -2878,10 +2911,10 @@
       <c r="CE6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="CF6" s="26" t="s">
+      <c r="CF6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="CG6" s="29" t="s">
+      <c r="CG6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="CH6" s="5" t="s">
@@ -2899,10 +2932,10 @@
       <c r="CL6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="CM6" s="26" t="s">
+      <c r="CM6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="CN6" s="29" t="s">
+      <c r="CN6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="CO6" s="5" t="s">
@@ -2920,19 +2953,19 @@
       <c r="CS6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="CT6" s="26" t="s">
+      <c r="CT6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="CU6" s="29" t="s">
+      <c r="CU6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="CV6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="CW6" s="5" t="s">
+      <c r="CW6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="CX6" s="5" t="s">
+      <c r="CX6" s="14" t="s">
         <v>3</v>
       </c>
       <c r="CY6" s="5" t="s">
@@ -2941,19 +2974,19 @@
       <c r="CZ6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="DA6" s="26" t="s">
+      <c r="DA6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="DB6" s="29" t="s">
+      <c r="DB6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="DC6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="DD6" s="14" t="s">
+      <c r="DD6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="DE6" s="14" t="s">
+      <c r="DE6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="DF6" s="5" t="s">
@@ -2962,49 +2995,31 @@
       <c r="DG6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="DH6" s="26" t="s">
+      <c r="DH6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="DI6" s="29" t="s">
+      <c r="DI6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="DJ6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="DK6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="DL6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="DM6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="DN6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="DO6" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="DP6" s="29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:120" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31" t="s">
+    </row>
+    <row r="7" spans="1:113" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="F7" s="37"/>
-    </row>
-    <row r="8" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="42"/>
+    </row>
+    <row r="8" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="7"/>
+      <c r="AS8" s="7"/>
+      <c r="AT8" s="7"/>
+      <c r="AU8" s="7"/>
       <c r="AV8" s="7"/>
-      <c r="AW8" s="7"/>
-      <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
       <c r="AZ8" s="7"/>
       <c r="BA8" s="7"/>
@@ -3020,16 +3035,16 @@
       <c r="BO8" s="7"/>
       <c r="BP8" s="7"/>
       <c r="BQ8" s="7"/>
-      <c r="BT8" s="7"/>
-      <c r="BU8" s="7"/>
-      <c r="BV8" s="7"/>
-      <c r="BW8" s="7"/>
-      <c r="BX8" s="7"/>
-    </row>
-    <row r="9" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
       <c r="AF9" s="7"/>
@@ -3040,13 +3055,13 @@
       <c r="AM9" s="7"/>
       <c r="AN9" s="7"/>
       <c r="AO9" s="7"/>
+      <c r="AP9" s="7"/>
+      <c r="AQ9" s="7"/>
       <c r="AR9" s="7"/>
       <c r="AS9" s="7"/>
       <c r="AT9" s="7"/>
       <c r="AU9" s="7"/>
       <c r="AV9" s="7"/>
-      <c r="AW9" s="7"/>
-      <c r="AX9" s="7"/>
       <c r="AY9" s="7"/>
       <c r="AZ9" s="7"/>
       <c r="BA9" s="7"/>
@@ -3057,386 +3072,265 @@
       <c r="BH9" s="7"/>
       <c r="BI9" s="7"/>
       <c r="BJ9" s="7"/>
-      <c r="BM9" s="7"/>
-      <c r="BN9" s="7"/>
-      <c r="BO9" s="7"/>
-      <c r="BP9" s="7"/>
-      <c r="BQ9" s="7"/>
-    </row>
-    <row r="10" spans="1:120" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
+    </row>
+    <row r="10" spans="1:113" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="43"/>
+    </row>
+    <row r="11" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="26"/>
+    </row>
+    <row r="12" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+    </row>
+    <row r="14" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="26"/>
+      <c r="AD14" s="26"/>
+      <c r="AE14" s="26"/>
+      <c r="AF14" s="26"/>
+      <c r="AG14" s="26"/>
+      <c r="AH14" s="26"/>
+      <c r="AK14" s="26"/>
+      <c r="AL14" s="26"/>
+      <c r="AM14" s="26"/>
+      <c r="AN14" s="26"/>
+      <c r="AO14" s="26"/>
+      <c r="AR14" s="26"/>
+      <c r="AS14" s="26"/>
+      <c r="AT14" s="26"/>
+      <c r="AU14" s="26"/>
+      <c r="AV14" s="26"/>
+      <c r="AY14" s="26"/>
+      <c r="AZ14" s="26"/>
+      <c r="BA14" s="26"/>
+      <c r="BB14" s="26"/>
+      <c r="BC14" s="26"/>
+    </row>
+    <row r="15" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="BF15" s="26"/>
+      <c r="BG15" s="26"/>
+      <c r="BH15" s="26"/>
+      <c r="BI15" s="26"/>
+      <c r="BJ15" s="26"/>
+    </row>
+    <row r="16" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:113" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="38"/>
-    </row>
-    <row r="11" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-    </row>
-    <row r="12" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-    </row>
-    <row r="13" spans="1:120" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="C19" s="42"/>
+    </row>
+    <row r="20" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="DD22" s="7"/>
+    </row>
+    <row r="23" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="28"/>
-      <c r="Z13" s="28"/>
-      <c r="AA13" s="28"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="27"/>
-      <c r="AD13" s="28"/>
-      <c r="AE13" s="28"/>
-      <c r="AF13" s="28"/>
-      <c r="AG13" s="28"/>
-      <c r="AH13" s="28"/>
-      <c r="AI13" s="27"/>
-      <c r="AJ13" s="27"/>
-      <c r="AP13" s="27"/>
-      <c r="AQ13" s="27"/>
-      <c r="AW13" s="27"/>
-      <c r="AX13" s="27"/>
-      <c r="BD13" s="27"/>
-      <c r="BE13" s="27"/>
-      <c r="BK13" s="27"/>
-      <c r="BL13" s="27"/>
-      <c r="BR13" s="27"/>
-      <c r="BS13" s="27"/>
-      <c r="BY13" s="27"/>
-      <c r="BZ13" s="27"/>
-      <c r="CF13" s="27"/>
-      <c r="CG13" s="27"/>
-      <c r="CM13" s="27"/>
-      <c r="CN13" s="27"/>
-      <c r="CT13" s="27"/>
-      <c r="CU13" s="27"/>
-      <c r="DA13" s="27"/>
-      <c r="DB13" s="27"/>
-      <c r="DD13" s="18"/>
-      <c r="DE13" s="18"/>
-      <c r="DH13" s="27"/>
-      <c r="DI13" s="27"/>
-      <c r="DK13" s="19"/>
-      <c r="DO13" s="27"/>
-      <c r="DP13" s="27"/>
-    </row>
-    <row r="14" spans="1:120" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    </row>
+    <row r="26" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:113" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="Y14" s="28"/>
-      <c r="Z14" s="28"/>
-      <c r="AA14" s="28"/>
-      <c r="AB14" s="27"/>
-      <c r="AC14" s="27"/>
-      <c r="AD14" s="28"/>
-      <c r="AE14" s="28"/>
-      <c r="AF14" s="28"/>
-      <c r="AG14" s="28"/>
-      <c r="AH14" s="28"/>
-      <c r="AI14" s="27"/>
-      <c r="AJ14" s="27"/>
-      <c r="AP14" s="27"/>
-      <c r="AQ14" s="27"/>
-      <c r="AW14" s="27"/>
-      <c r="AX14" s="27"/>
-      <c r="BD14" s="27"/>
-      <c r="BE14" s="27"/>
-      <c r="BK14" s="27"/>
-      <c r="BL14" s="27"/>
-      <c r="BR14" s="27"/>
-      <c r="BS14" s="27"/>
-      <c r="BY14" s="27"/>
-      <c r="BZ14" s="27"/>
-      <c r="CF14" s="27"/>
-      <c r="CG14" s="27"/>
-      <c r="CM14" s="27"/>
-      <c r="CN14" s="27"/>
-      <c r="CT14" s="27"/>
-      <c r="CU14" s="27"/>
-      <c r="DA14" s="27"/>
-      <c r="DB14" s="27"/>
-      <c r="DD14" s="18"/>
-      <c r="DE14" s="18"/>
-      <c r="DH14" s="27"/>
-      <c r="DI14" s="27"/>
-      <c r="DK14" s="19"/>
-      <c r="DO14" s="27"/>
-      <c r="DP14" s="27"/>
-    </row>
-    <row r="15" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK15" s="22"/>
-      <c r="AL15" s="22"/>
-      <c r="AM15" s="22"/>
-      <c r="AN15" s="22"/>
-      <c r="AO15" s="22"/>
-      <c r="AR15" s="22"/>
-      <c r="AS15" s="22"/>
-      <c r="AT15" s="22"/>
-      <c r="AU15" s="22"/>
-      <c r="AV15" s="22"/>
-    </row>
-    <row r="16" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="W16" s="22"/>
-      <c r="X16" s="22"/>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="22"/>
-      <c r="AA16" s="22"/>
-      <c r="AD16" s="22"/>
-      <c r="AE16" s="22"/>
-      <c r="AF16" s="22"/>
-      <c r="AG16" s="22"/>
-      <c r="AH16" s="22"/>
-      <c r="AK16" s="22"/>
-      <c r="AL16" s="22"/>
-      <c r="AM16" s="22"/>
-      <c r="AN16" s="22"/>
-      <c r="AO16" s="22"/>
-      <c r="AR16" s="22"/>
-      <c r="AS16" s="22"/>
-      <c r="AT16" s="22"/>
-      <c r="AU16" s="22"/>
-      <c r="AV16" s="22"/>
-      <c r="AY16" s="22"/>
-      <c r="AZ16" s="22"/>
-      <c r="BA16" s="22"/>
-      <c r="BB16" s="22"/>
-      <c r="BC16" s="22"/>
-    </row>
-    <row r="17" spans="1:83" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
+      <c r="C27" s="42"/>
+    </row>
+    <row r="28" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR28" s="26"/>
+      <c r="AS28" s="26"/>
+      <c r="AT28" s="26"/>
+      <c r="AU28" s="26"/>
+      <c r="AV28" s="26"/>
+      <c r="AY28" s="26"/>
+      <c r="AZ28" s="26"/>
+      <c r="BA28" s="26"/>
+      <c r="BB28" s="26"/>
+      <c r="BC28" s="26"/>
+    </row>
+    <row r="29" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="38"/>
-    </row>
-    <row r="24" spans="1:83" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="37"/>
-    </row>
-    <row r="25" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>35</v>
-      </c>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-    </row>
-    <row r="26" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>36</v>
-      </c>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-    </row>
-    <row r="27" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    </row>
+    <row r="30" spans="1:113" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="N30" s="37"/>
+      <c r="O30" s="37"/>
+      <c r="U30" s="37"/>
+      <c r="V30" s="37"/>
+      <c r="AB30" s="37"/>
+      <c r="AC30" s="37"/>
+      <c r="AI30" s="37"/>
+      <c r="AJ30" s="37"/>
+      <c r="AP30" s="37"/>
+      <c r="AQ30" s="37"/>
+      <c r="AW30" s="37"/>
+      <c r="AX30" s="37"/>
+      <c r="BD30" s="37"/>
+      <c r="BE30" s="37"/>
+      <c r="BK30" s="37"/>
+      <c r="BL30" s="37"/>
+      <c r="BR30" s="37"/>
+      <c r="BS30" s="37"/>
+      <c r="BY30" s="37"/>
+      <c r="BZ30" s="37"/>
+      <c r="CF30" s="37"/>
+      <c r="CG30" s="37"/>
+      <c r="CM30" s="37"/>
+      <c r="CN30" s="37"/>
+      <c r="CT30" s="37"/>
+      <c r="CU30" s="37"/>
+      <c r="CW30" s="39"/>
+      <c r="CX30" s="39"/>
+      <c r="DA30" s="37"/>
+      <c r="DB30" s="37"/>
+      <c r="DD30" s="38"/>
+      <c r="DH30" s="37"/>
+      <c r="DI30" s="37"/>
+    </row>
+    <row r="31" spans="1:113" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:113" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="42"/>
+    </row>
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22"/>
-      <c r="U27" s="22"/>
-    </row>
-    <row r="28" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="W28" s="22"/>
-      <c r="X28" s="22"/>
-      <c r="Y28" s="22"/>
-      <c r="Z28" s="22"/>
-      <c r="AA28" s="22"/>
-      <c r="AB28" s="22"/>
-      <c r="AC28" s="22"/>
-      <c r="AD28" s="22"/>
-      <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="22"/>
-      <c r="AH28" s="22"/>
-    </row>
-    <row r="29" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK29" s="22"/>
-      <c r="AL29" s="22"/>
-      <c r="AM29" s="22"/>
-      <c r="AN29" s="22"/>
-      <c r="AO29" s="22"/>
-    </row>
-    <row r="30" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR30" s="22"/>
-      <c r="AS30" s="22"/>
-      <c r="AT30" s="22"/>
-      <c r="AU30" s="22"/>
-      <c r="AV30" s="22"/>
-      <c r="AW30" s="22"/>
-      <c r="AX30" s="22"/>
-      <c r="AY30" s="22"/>
-      <c r="AZ30" s="22"/>
-      <c r="BA30" s="22"/>
-      <c r="BB30" s="22"/>
-      <c r="BC30" s="22"/>
-      <c r="BD30" s="22"/>
-      <c r="BE30" s="22"/>
-      <c r="BF30" s="22"/>
-      <c r="BG30" s="22"/>
-      <c r="BH30" s="22"/>
-      <c r="BI30" s="22"/>
-      <c r="BJ30" s="22"/>
-      <c r="BK30" s="22"/>
-      <c r="BL30" s="22"/>
-      <c r="BM30" s="22"/>
-      <c r="BN30" s="22"/>
-      <c r="BO30" s="22"/>
-      <c r="BP30" s="22"/>
-      <c r="BQ30" s="22"/>
-      <c r="BR30" s="22"/>
-      <c r="BS30" s="22"/>
-      <c r="BT30" s="22"/>
-      <c r="BU30" s="22"/>
-      <c r="BV30" s="22"/>
-      <c r="BW30" s="22"/>
-      <c r="BX30" s="22"/>
-      <c r="BY30" s="22"/>
-      <c r="BZ30" s="22"/>
-      <c r="CA30" s="22"/>
-      <c r="CB30" s="22"/>
-      <c r="CC30" s="22"/>
-      <c r="CD30" s="22"/>
-      <c r="CE30" s="22"/>
-    </row>
-    <row r="31" spans="1:83" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="43"/>
-      <c r="T31" s="43"/>
-      <c r="U31" s="43"/>
-      <c r="V31" s="43"/>
-      <c r="W31" s="43"/>
-      <c r="X31" s="43"/>
-      <c r="Y31" s="43"/>
-      <c r="Z31" s="43"/>
-      <c r="AA31" s="43"/>
-      <c r="AB31" s="43"/>
-      <c r="AC31" s="43"/>
-      <c r="AD31" s="43"/>
-      <c r="AE31" s="43"/>
-      <c r="AF31" s="43"/>
-      <c r="AG31" s="43"/>
-      <c r="AH31" s="43"/>
-      <c r="AI31" s="43"/>
-      <c r="AJ31" s="43"/>
-      <c r="AK31" s="43"/>
-      <c r="AL31" s="43"/>
-      <c r="AM31" s="43"/>
-      <c r="AN31" s="43"/>
-      <c r="AO31" s="43"/>
-      <c r="AP31" s="43"/>
-      <c r="AQ31" s="43"/>
-      <c r="AR31" s="43"/>
-      <c r="AS31" s="43"/>
-      <c r="AT31" s="43"/>
-      <c r="AU31" s="43"/>
-      <c r="AV31" s="43"/>
-      <c r="AW31" s="43"/>
-      <c r="AX31" s="43"/>
-      <c r="AY31" s="43"/>
-      <c r="AZ31" s="43"/>
-      <c r="BA31" s="43"/>
-      <c r="BB31" s="43"/>
-      <c r="BC31" s="43"/>
-      <c r="BD31" s="43"/>
-      <c r="BE31" s="43"/>
-      <c r="BF31" s="43"/>
-      <c r="BG31" s="43"/>
-      <c r="BH31" s="43"/>
-      <c r="BI31" s="43"/>
-      <c r="BJ31" s="43"/>
-      <c r="BK31" s="43"/>
-      <c r="BL31" s="43"/>
-      <c r="BM31" s="43"/>
-      <c r="BN31" s="43"/>
-      <c r="BO31" s="43"/>
-      <c r="BP31" s="43"/>
-      <c r="BQ31" s="43"/>
-      <c r="BR31" s="43"/>
-      <c r="BS31" s="43"/>
-      <c r="BT31" s="43"/>
-      <c r="BU31" s="43"/>
-      <c r="BV31" s="43"/>
-      <c r="BW31" s="43"/>
-      <c r="BX31" s="43"/>
-      <c r="BY31" s="43"/>
-      <c r="BZ31" s="43"/>
-      <c r="CA31" s="43"/>
-      <c r="CB31" s="43"/>
-      <c r="CC31" s="43"/>
-      <c r="CD31" s="43"/>
-      <c r="CE31" s="43"/>
-    </row>
-    <row r="32" spans="1:83" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="38"/>
+    </row>
+    <row r="42" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="36" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="CA4:CG4"/>
+  <mergeCells count="16">
+    <mergeCell ref="BT4:BZ4"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -3447,12 +3341,11 @@
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.78740157480314965" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3464,6 +3357,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D98DF252718B14F9C13E50871EB3D76" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="33c83fdbb9e9dd0c2649960876b7423f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0" xmlns:ns3="909da4c9-3531-4fb4-a16c-fe746456455a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ab13681565d5f0eb6f0b0e10da5abf3" ns2:_="" ns3:_="">
     <xsd:import namespace="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0"/>
@@ -3691,7 +3643,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0">0-93518095-55993</_dlc_DocId>
@@ -3703,66 +3655,23 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1376E91E-7564-4EA7-82E9-F45D5BE229A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E01570BF-52F9-46B8-9C85-26D2F1ECBEF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6ACD257-8FA8-4D4D-8960-D1074C7DEC25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3781,7 +3690,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC31D3A6-4EB4-4E27-A5DB-8C0892094121}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3791,18 +3700,8 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1376E91E-7564-4EA7-82E9-F45D5BE229A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E01570BF-52F9-46B8-9C85-26D2F1ECBEF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{fe4bc684-102f-461d-a6dc-b1e58752f380}" enabled="1" method="Standard" siteId="{2d75a51b-29e5-45d5-a5c5-5aa979cb6a28}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
final gant chart upload
</commit_message>
<xml_diff>
--- a/docs/gantt_chart_secrecy.xlsx
+++ b/docs/gantt_chart_secrecy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mimoun.mendoughe/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evonik-my.sharepoint.com/personal/d23031_evonik_com/Documents/Dokumente/personal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FBB666-BCE3-7846-9B67-C5A62DD59BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{06D75C9C-9DE6-4893-9567-56061F415DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" xr2:uid="{D30480B8-D58C-44F1-852C-2B52D77C9917}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D30480B8-D58C-44F1-852C-2B52D77C9917}"/>
   </bookViews>
   <sheets>
     <sheet name="Mappe 1" sheetId="2" r:id="rId1"/>
@@ -213,10 +213,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;€&quot;* #,##0.00_);_(&quot;€&quot;* \(#,##0.00\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;€&quot;* #,##0_);_(&quot;€&quot;* \(#,##0\);_(&quot;€&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;€&quot;* #,##0.00_);_(&quot;€&quot;* \(#,##0.00\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -535,7 +535,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -700,13 +700,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
@@ -736,7 +745,7 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -829,6 +838,19 @@
     <xf numFmtId="0" fontId="17" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Accent1" xfId="22" builtinId="29" customBuiltin="1"/>
@@ -1682,11 +1704,11 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFCCFF99"/>
       <color rgb="FF99CCFF"/>
       <color rgb="FFFF5050"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FFCCECFF"/>
-      <color rgb="FFCCFF99"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFFF9966"/>
     </mruColors>
@@ -2103,82 +2125,83 @@
   </sheetPr>
   <dimension ref="A1:DI42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK31" sqref="AK31:AO31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="7.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="1.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="34" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="41" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="44" max="47" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="1.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="1.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="58" max="62" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="65" max="69" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="72" max="76" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="77" max="78" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="84" max="85" width="1.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="88" max="90" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="91" max="92" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="93" max="97" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="98" max="99" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="101" max="102" width="2.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="103" max="104" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="105" max="106" width="2.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="2.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="1.42578125" bestFit="1" customWidth="1"/>
-    <col min="112" max="113" width="1.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1796875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="1.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="1.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="34" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="37" max="41" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="44" max="47" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="1.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="1.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="1.453125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="1.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="58" max="62" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="65" max="69" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="72" max="76" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="1.453125" bestFit="1" customWidth="1"/>
+    <col min="84" max="85" width="1.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="88" max="90" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="91" max="92" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="93" max="97" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="98" max="99" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="101" max="102" width="2.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="103" max="104" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="105" max="106" width="2.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="2.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="1.54296875" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="1.453125" bestFit="1" customWidth="1"/>
+    <col min="112" max="113" width="1.54296875" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
       <c r="CW1"/>
       <c r="CX1"/>
       <c r="DD1"/>
     </row>
-    <row r="2" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -2186,13 +2209,13 @@
       <c r="CX2"/>
       <c r="DD2"/>
     </row>
-    <row r="3" spans="1:113" ht="19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:113" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="CW3"/>
       <c r="CX3"/>
       <c r="DD3"/>
     </row>
-    <row r="4" spans="1:113" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:113" ht="29.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="43" t="s">
         <v>11</v>
@@ -2339,15 +2362,15 @@
       <c r="DH4" s="44"/>
       <c r="DI4" s="45"/>
     </row>
-    <row r="5" spans="1:113" ht="19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:113" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="3">
         <v>16</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="48">
         <v>17</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="24">
         <v>18</v>
       </c>
       <c r="E5" s="2">
@@ -2663,18 +2686,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:113" ht="19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:113" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -3002,13 +3025,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:113" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:113" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="39"/>
-    </row>
-    <row r="8" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="49"/>
+      <c r="D7" s="39"/>
+    </row>
+    <row r="8" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3036,7 +3060,7 @@
       <c r="BP8" s="7"/>
       <c r="BQ8" s="7"/>
     </row>
-    <row r="9" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3073,29 +3097,30 @@
       <c r="BI9" s="7"/>
       <c r="BJ9" s="7"/>
     </row>
-    <row r="10" spans="1:113" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:113" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="40"/>
-    </row>
-    <row r="11" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="50"/>
+      <c r="D10" s="40"/>
+    </row>
+    <row r="11" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="26"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="26"/>
-    </row>
-    <row r="12" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="51"/>
+      <c r="D11" s="42"/>
+    </row>
+    <row r="12" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="26"/>
       <c r="F12" s="26"/>
     </row>
-    <row r="13" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>30</v>
       </c>
@@ -3113,7 +3138,7 @@
       <c r="X13" s="26"/>
       <c r="Y13" s="26"/>
     </row>
-    <row r="14" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>35</v>
       </c>
@@ -3143,7 +3168,7 @@
       <c r="BB14" s="26"/>
       <c r="BC14" s="26"/>
     </row>
-    <row r="15" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>43</v>
       </c>
@@ -3153,7 +3178,7 @@
       <c r="BI15" s="26"/>
       <c r="BJ15" s="26"/>
     </row>
-    <row r="16" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>34</v>
       </c>
@@ -3163,7 +3188,7 @@
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
     </row>
-    <row r="17" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>26</v>
       </c>
@@ -3172,39 +3197,90 @@
       <c r="N17" s="32"/>
       <c r="O17" s="32"/>
     </row>
-    <row r="18" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:113" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:113" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="39"/>
-    </row>
-    <row r="20" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="49"/>
+      <c r="D19" s="39"/>
+    </row>
+    <row r="20" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="31"/>
+      <c r="Z20" s="31"/>
+      <c r="AA20" s="31"/>
+      <c r="AR20" s="31"/>
+      <c r="AS20" s="31"/>
+      <c r="AT20" s="31"/>
+      <c r="AU20" s="31"/>
+      <c r="AV20" s="31"/>
+      <c r="AY20" s="31"/>
+      <c r="AZ20" s="31"/>
+      <c r="BA20" s="31"/>
+      <c r="BB20" s="31"/>
+      <c r="BC20" s="31"/>
+      <c r="BF20" s="31"/>
+      <c r="BG20" s="31"/>
+      <c r="BH20" s="31"/>
+      <c r="BI20" s="31"/>
+      <c r="BJ20" s="31"/>
+    </row>
+    <row r="21" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="31"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+    </row>
+    <row r="22" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>53</v>
       </c>
+      <c r="AD22" s="31"/>
+      <c r="AE22" s="31"/>
+      <c r="AF22" s="31"/>
+      <c r="AG22" s="31"/>
+      <c r="AH22" s="31"/>
+      <c r="AK22" s="31"/>
+      <c r="AL22" s="31"/>
+      <c r="AM22" s="31"/>
+      <c r="AN22" s="31"/>
+      <c r="AO22" s="31"/>
       <c r="DD22" s="7"/>
     </row>
-    <row r="23" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>38</v>
       </c>
@@ -3217,7 +3293,7 @@
       <c r="Z24" s="32"/>
       <c r="AA24" s="32"/>
     </row>
-    <row r="25" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>27</v>
       </c>
@@ -3227,18 +3303,19 @@
       <c r="AG25" s="32"/>
       <c r="AH25" s="32"/>
     </row>
-    <row r="26" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:113" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:113" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="39"/>
-    </row>
-    <row r="28" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="49"/>
+      <c r="D27" s="39"/>
+    </row>
+    <row r="28" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>42</v>
       </c>
@@ -3253,16 +3330,17 @@
       <c r="BB28" s="26"/>
       <c r="BC28" s="26"/>
     </row>
-    <row r="29" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:113" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:113" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="29"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="29"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
       <c r="N30" s="34"/>
@@ -3299,7 +3377,7 @@
       <c r="DH30" s="34"/>
       <c r="DI30" s="34"/>
     </row>
-    <row r="31" spans="1:113" ht="19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:113" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>41</v>
       </c>
@@ -3309,59 +3387,55 @@
       <c r="AN31" s="32"/>
       <c r="AO31" s="32"/>
     </row>
-    <row r="32" spans="1:113" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:113" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="39"/>
-    </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="49"/>
+      <c r="D32" s="39"/>
+    </row>
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="33" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="BT4:BZ4"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="I4:O4"/>
@@ -3373,38 +3447,22 @@
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.78740157480314965" header="0.39370078740157483" footer="0.39370078740157483"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;9&amp;D&amp;R&amp;9Seite &amp;P</oddFooter>
+    <oddFooter>&amp;L&amp;9&amp;D_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 [confidential]&amp;R&amp;9Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0">0-93518095-55993</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0">
-      <Url>https://evonik.sharepoint.com/sites/13129/_layouts/15/DocIdRedir.aspx?ID=0-93518095-55993</Url>
-      <Description>0-93518095-55993</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D98DF252718B14F9C13E50871EB3D76" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="33c83fdbb9e9dd0c2649960876b7423f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0" xmlns:ns3="909da4c9-3531-4fb4-a16c-fe746456455a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ab13681565d5f0eb6f0b0e10da5abf3" ns2:_="" ns3:_="">
     <xsd:import namespace="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0"/>
@@ -3632,6 +3690,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0">0-93518095-55993</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0">
+      <Url>https://evonik.sharepoint.com/sites/13129/_layouts/15/DocIdRedir.aspx?ID=0-93518095-55993</Url>
+      <Description>0-93518095-55993</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -3683,24 +3762,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1376E91E-7564-4EA7-82E9-F45D5BE229A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC31D3A6-4EB4-4E27-A5DB-8C0892094121}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6ACD257-8FA8-4D4D-8960-D1074C7DEC25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3719,6 +3780,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC31D3A6-4EB4-4E27-A5DB-8C0892094121}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e1e3eed4-e974-45e8-a8bb-c4e1c86ee8e0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1376E91E-7564-4EA7-82E9-F45D5BE229A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E01570BF-52F9-46B8-9C85-26D2F1ECBEF4}">
   <ds:schemaRefs>

</xml_diff>